<commit_message>
Update to match all regions
</commit_message>
<xml_diff>
--- a/CCMA.xlsx
+++ b/CCMA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\Descarga_CCMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F736C125-FC6B-4716-8E1B-08477691C411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADAE758-D20D-420A-BD13-3A01D9B6A90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1800,7 +1800,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1887,14 +1887,14 @@
       </c>
       <c r="F2" s="3">
         <f ca="1">TODAY()</f>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A2,"0")," - ","CCMA - ",TEXT(F2,"AAAAMM")," - ",SUBSTITUTE(D2,"-","")," - ",B2)</f>
-        <v>0 - CCMA - 202304 - 20000000000 - Cliente</v>
+        <f ca="1">CONCATENATE(TEXT(A2,"0")," - ","CCMA - ",YEAR(F2)&amp;TEXT(MONTH(F2),"00")," - ",SUBSTITUTE(D2,"-","")," - ",B2)</f>
+        <v>0 - CCMA - 202307 - 20000000000 - Cliente</v>
       </c>
       <c r="K2" s="4" t="e">
         <f>VLOOKUP(C2,[1]Hoja1!$J:$L,3,0)</f>
@@ -1909,15 +1909,15 @@
         <v>2</v>
       </c>
       <c r="N2" s="4">
-        <f t="shared" ref="N2:N33" si="3">IF(C2=C1,1,0)</f>
+        <f t="shared" ref="N2" si="3">IF(C2=C1,1,0)</f>
         <v>0</v>
       </c>
       <c r="O2" s="4">
-        <f t="shared" ref="O2:O33" si="4">IF(C2=C3,1,0)</f>
+        <f t="shared" ref="O2" si="4">IF(C2=C3,1,0)</f>
         <v>1</v>
       </c>
       <c r="P2" s="4">
-        <f t="shared" ref="P2:P33" si="5">SUM(N2:O2)</f>
+        <f t="shared" ref="P2" si="5">SUM(N2:O2)</f>
         <v>1</v>
       </c>
     </row>
@@ -1941,14 +1941,14 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F66" ca="1" si="6">TODAY()</f>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="2" t="str">
-        <f t="shared" ref="J3:J66" ca="1" si="7">CONCATENATE(TEXT(A3,"0")," - ","CCMA - ",TEXT(F3,"AAAAMM")," - ",SUBSTITUTE(D3,"-","")," - ",B3)</f>
-        <v>0 - CCMA - 202304 - 20000000000 - Cliente</v>
+        <f t="shared" ref="J3:J66" ca="1" si="7">CONCATENATE(TEXT(A3,"0")," - ","CCMA - ",YEAR(F3)&amp;TEXT(MONTH(F3),"00")," - ",SUBSTITUTE(D3,"-","")," - ",B3)</f>
+        <v>0 - CCMA - 202307 - 20000000000 - Cliente</v>
       </c>
       <c r="K3" s="4" t="e">
         <f>VLOOKUP(C3,[1]Hoja1!$J:$L,3,0)</f>
@@ -1994,14 +1994,14 @@
       </c>
       <c r="F4" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K4" s="4" t="e">
         <f>VLOOKUP(C4,[1]Hoja1!$J:$L,3,0)</f>
@@ -2047,14 +2047,14 @@
       </c>
       <c r="F5" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K5" s="4" t="e">
         <f>VLOOKUP(C5,[1]Hoja1!$J:$L,3,0)</f>
@@ -2100,14 +2100,14 @@
       </c>
       <c r="F6" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K6" s="4" t="e">
         <f>VLOOKUP(C6,[1]Hoja1!$J:$L,3,0)</f>
@@ -2153,14 +2153,14 @@
       </c>
       <c r="F7" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K7" s="4" t="e">
         <f>VLOOKUP(C7,[1]Hoja1!$J:$L,3,0)</f>
@@ -2206,14 +2206,14 @@
       </c>
       <c r="F8" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K8" s="4" t="e">
         <f>VLOOKUP(C8,[1]Hoja1!$J:$L,3,0)</f>
@@ -2259,14 +2259,14 @@
       </c>
       <c r="F9" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K9" s="4" t="e">
         <f>VLOOKUP(C9,[1]Hoja1!$J:$L,3,0)</f>
@@ -2312,14 +2312,14 @@
       </c>
       <c r="F10" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K10" s="4" t="e">
         <f>VLOOKUP(C10,[1]Hoja1!$J:$L,3,0)</f>
@@ -2365,14 +2365,14 @@
       </c>
       <c r="F11" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K11" s="4" t="e">
         <f>VLOOKUP(C11,[1]Hoja1!$J:$L,3,0)</f>
@@ -2418,14 +2418,14 @@
       </c>
       <c r="F12" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K12" s="4" t="e">
         <f>VLOOKUP(C12,[1]Hoja1!$J:$L,3,0)</f>
@@ -2471,14 +2471,14 @@
       </c>
       <c r="F13" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K13" s="4" t="e">
         <f>VLOOKUP(C13,[1]Hoja1!$J:$L,3,0)</f>
@@ -2524,14 +2524,14 @@
       </c>
       <c r="F14" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K14" s="4" t="e">
         <f>VLOOKUP(C14,[1]Hoja1!$J:$L,3,0)</f>
@@ -2577,14 +2577,14 @@
       </c>
       <c r="F15" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K15" s="4" t="e">
         <f>VLOOKUP(C15,[1]Hoja1!$J:$L,3,0)</f>
@@ -2630,14 +2630,14 @@
       </c>
       <c r="F16" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K16" s="4" t="e">
         <f>VLOOKUP(C16,[1]Hoja1!$J:$L,3,0)</f>
@@ -2683,14 +2683,14 @@
       </c>
       <c r="F17" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K17" s="4" t="e">
         <f>VLOOKUP(C17,[1]Hoja1!$J:$L,3,0)</f>
@@ -2736,14 +2736,14 @@
       </c>
       <c r="F18" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K18" s="4" t="e">
         <f>VLOOKUP(C18,[1]Hoja1!$J:$L,3,0)</f>
@@ -2789,14 +2789,14 @@
       </c>
       <c r="F19" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K19" s="4" t="e">
         <f>VLOOKUP(C19,[1]Hoja1!$J:$L,3,0)</f>
@@ -2842,14 +2842,14 @@
       </c>
       <c r="F20" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K20" s="4" t="e">
         <f>VLOOKUP(C20,[1]Hoja1!$J:$L,3,0)</f>
@@ -2895,14 +2895,14 @@
       </c>
       <c r="F21" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K21" s="4" t="e">
         <f>VLOOKUP(C21,[1]Hoja1!$J:$L,3,0)</f>
@@ -2948,14 +2948,14 @@
       </c>
       <c r="F22" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K22" s="4" t="e">
         <f>VLOOKUP(C22,[1]Hoja1!$J:$L,3,0)</f>
@@ -3001,14 +3001,14 @@
       </c>
       <c r="F23" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K23" s="4" t="e">
         <f>VLOOKUP(C23,[1]Hoja1!$J:$L,3,0)</f>
@@ -3054,14 +3054,14 @@
       </c>
       <c r="F24" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K24" s="4" t="e">
         <f>VLOOKUP(C24,[1]Hoja1!$J:$L,3,0)</f>
@@ -3107,14 +3107,14 @@
       </c>
       <c r="F25" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K25" s="4" t="e">
         <f>VLOOKUP(C25,[1]Hoja1!$J:$L,3,0)</f>
@@ -3160,14 +3160,14 @@
       </c>
       <c r="F26" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K26" s="4" t="e">
         <f>VLOOKUP(C26,[1]Hoja1!$J:$L,3,0)</f>
@@ -3213,14 +3213,14 @@
       </c>
       <c r="F27" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K27" s="4" t="e">
         <f>VLOOKUP(C27,[1]Hoja1!$J:$L,3,0)</f>
@@ -3266,14 +3266,14 @@
       </c>
       <c r="F28" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K28" s="4" t="e">
         <f>VLOOKUP(C28,[1]Hoja1!$J:$L,3,0)</f>
@@ -3319,14 +3319,14 @@
       </c>
       <c r="F29" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K29" s="4" t="e">
         <f>VLOOKUP(C29,[1]Hoja1!$J:$L,3,0)</f>
@@ -3372,14 +3372,14 @@
       </c>
       <c r="F30" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K30" s="4" t="e">
         <f>VLOOKUP(C30,[1]Hoja1!$J:$L,3,0)</f>
@@ -3425,14 +3425,14 @@
       </c>
       <c r="F31" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K31" s="4" t="e">
         <f>VLOOKUP(C31,[1]Hoja1!$J:$L,3,0)</f>
@@ -3478,14 +3478,14 @@
       </c>
       <c r="F32" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K32" s="4" t="e">
         <f>VLOOKUP(C32,[1]Hoja1!$J:$L,3,0)</f>
@@ -3531,14 +3531,14 @@
       </c>
       <c r="F33" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K33" s="4" t="e">
         <f>VLOOKUP(C33,[1]Hoja1!$J:$L,3,0)</f>
@@ -3584,14 +3584,14 @@
       </c>
       <c r="F34" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K34" s="4" t="e">
         <f>VLOOKUP(C34,[1]Hoja1!$J:$L,3,0)</f>
@@ -3637,14 +3637,14 @@
       </c>
       <c r="F35" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="J35" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K35" s="4" t="e">
         <f>VLOOKUP(C35,[1]Hoja1!$J:$L,3,0)</f>
@@ -3690,14 +3690,14 @@
       </c>
       <c r="F36" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="J36" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K36" s="4" t="e">
         <f>VLOOKUP(C36,[1]Hoja1!$J:$L,3,0)</f>
@@ -3743,14 +3743,14 @@
       </c>
       <c r="F37" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K37" s="4" t="e">
         <f>VLOOKUP(C37,[1]Hoja1!$J:$L,3,0)</f>
@@ -3796,14 +3796,14 @@
       </c>
       <c r="F38" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
       <c r="J38" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K38" s="4" t="e">
         <f>VLOOKUP(C38,[1]Hoja1!$J:$L,3,0)</f>
@@ -3849,14 +3849,14 @@
       </c>
       <c r="F39" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
       <c r="J39" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K39" s="4" t="e">
         <f>VLOOKUP(C39,[1]Hoja1!$J:$L,3,0)</f>
@@ -3902,14 +3902,14 @@
       </c>
       <c r="F40" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="J40" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K40" s="4" t="e">
         <f>VLOOKUP(C40,[1]Hoja1!$J:$L,3,0)</f>
@@ -3955,14 +3955,14 @@
       </c>
       <c r="F41" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="J41" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K41" s="4" t="e">
         <f>VLOOKUP(C41,[1]Hoja1!$J:$L,3,0)</f>
@@ -4008,14 +4008,14 @@
       </c>
       <c r="F42" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
       <c r="J42" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K42" s="4" t="e">
         <f>VLOOKUP(C42,[1]Hoja1!$J:$L,3,0)</f>
@@ -4061,14 +4061,14 @@
       </c>
       <c r="F43" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K43" s="4" t="e">
         <f>VLOOKUP(C43,[1]Hoja1!$J:$L,3,0)</f>
@@ -4114,14 +4114,14 @@
       </c>
       <c r="F44" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
       <c r="J44" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K44" s="4" t="e">
         <f>VLOOKUP(C44,[1]Hoja1!$J:$L,3,0)</f>
@@ -4167,14 +4167,14 @@
       </c>
       <c r="F45" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="J45" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K45" s="4" t="e">
         <f>VLOOKUP(C45,[1]Hoja1!$J:$L,3,0)</f>
@@ -4220,14 +4220,14 @@
       </c>
       <c r="F46" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="J46" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K46" s="4" t="e">
         <f>VLOOKUP(C46,[1]Hoja1!$J:$L,3,0)</f>
@@ -4273,14 +4273,14 @@
       </c>
       <c r="F47" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="J47" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K47" s="4" t="e">
         <f>VLOOKUP(C47,[1]Hoja1!$J:$L,3,0)</f>
@@ -4326,14 +4326,14 @@
       </c>
       <c r="F48" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="J48" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K48" s="4" t="e">
         <f>VLOOKUP(C48,[1]Hoja1!$J:$L,3,0)</f>
@@ -4379,14 +4379,14 @@
       </c>
       <c r="F49" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="J49" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K49" s="4" t="e">
         <f>VLOOKUP(C49,[1]Hoja1!$J:$L,3,0)</f>
@@ -4432,14 +4432,14 @@
       </c>
       <c r="F50" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="J50" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K50" s="4" t="e">
         <f>VLOOKUP(C50,[1]Hoja1!$J:$L,3,0)</f>
@@ -4485,14 +4485,14 @@
       </c>
       <c r="F51" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
       <c r="J51" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K51" s="4" t="e">
         <f>VLOOKUP(C51,[1]Hoja1!$J:$L,3,0)</f>
@@ -4538,14 +4538,14 @@
       </c>
       <c r="F52" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K52" s="4" t="e">
         <f>VLOOKUP(C52,[1]Hoja1!$J:$L,3,0)</f>
@@ -4591,14 +4591,14 @@
       </c>
       <c r="F53" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K53" s="4" t="e">
         <f>VLOOKUP(C53,[1]Hoja1!$J:$L,3,0)</f>
@@ -4644,14 +4644,14 @@
       </c>
       <c r="F54" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K54" s="4" t="e">
         <f>VLOOKUP(C54,[1]Hoja1!$J:$L,3,0)</f>
@@ -4697,14 +4697,14 @@
       </c>
       <c r="F55" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="J55" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K55" s="4" t="e">
         <f>VLOOKUP(C55,[1]Hoja1!$J:$L,3,0)</f>
@@ -4750,14 +4750,14 @@
       </c>
       <c r="F56" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
       <c r="J56" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K56" s="4" t="e">
         <f>VLOOKUP(C56,[1]Hoja1!$J:$L,3,0)</f>
@@ -4803,14 +4803,14 @@
       </c>
       <c r="F57" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
       <c r="J57" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K57" s="4" t="e">
         <f>VLOOKUP(C57,[1]Hoja1!$J:$L,3,0)</f>
@@ -4856,14 +4856,14 @@
       </c>
       <c r="F58" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
       <c r="J58" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K58" s="4" t="e">
         <f>VLOOKUP(C58,[1]Hoja1!$J:$L,3,0)</f>
@@ -4909,14 +4909,14 @@
       </c>
       <c r="F59" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
       <c r="J59" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K59" s="4" t="e">
         <f>VLOOKUP(C59,[1]Hoja1!$J:$L,3,0)</f>
@@ -4962,14 +4962,14 @@
       </c>
       <c r="F60" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
       <c r="J60" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K60" s="4" t="e">
         <f>VLOOKUP(C60,[1]Hoja1!$J:$L,3,0)</f>
@@ -5015,14 +5015,14 @@
       </c>
       <c r="F61" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
       <c r="J61" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K61" s="4" t="e">
         <f>VLOOKUP(C61,[1]Hoja1!$J:$L,3,0)</f>
@@ -5068,14 +5068,14 @@
       </c>
       <c r="F62" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
       <c r="J62" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K62" s="4" t="e">
         <f>VLOOKUP(C62,[1]Hoja1!$J:$L,3,0)</f>
@@ -5121,14 +5121,14 @@
       </c>
       <c r="F63" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
       <c r="J63" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K63" s="4" t="e">
         <f>VLOOKUP(C63,[1]Hoja1!$J:$L,3,0)</f>
@@ -5174,14 +5174,14 @@
       </c>
       <c r="F64" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
       <c r="J64" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K64" s="4" t="e">
         <f>VLOOKUP(C64,[1]Hoja1!$J:$L,3,0)</f>
@@ -5227,14 +5227,14 @@
       </c>
       <c r="F65" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
       <c r="J65" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K65" s="4" t="e">
         <f>VLOOKUP(C65,[1]Hoja1!$J:$L,3,0)</f>
@@ -5280,14 +5280,14 @@
       </c>
       <c r="F66" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
       <c r="J66" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K66" s="4" t="e">
         <f>VLOOKUP(C66,[1]Hoja1!$J:$L,3,0)</f>
@@ -5333,14 +5333,14 @@
       </c>
       <c r="F67" s="3">
         <f t="shared" ref="F67:F69" ca="1" si="15">TODAY()</f>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
       <c r="J67" s="2" t="str">
-        <f t="shared" ref="J67:J69" ca="1" si="16">CONCATENATE(TEXT(A67,"0")," - ","CCMA - ",TEXT(F67,"AAAAMM")," - ",SUBSTITUTE(D67,"-","")," - ",B67)</f>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <f t="shared" ref="J67:J69" ca="1" si="16">CONCATENATE(TEXT(A67,"0")," - ","CCMA - ",YEAR(F67)&amp;TEXT(MONTH(F67),"00")," - ",SUBSTITUTE(D67,"-","")," - ",B67)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K67" s="4" t="e">
         <f>VLOOKUP(C67,[1]Hoja1!$J:$L,3,0)</f>
@@ -5386,14 +5386,14 @@
       </c>
       <c r="F68" s="3">
         <f t="shared" ca="1" si="15"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
       <c r="J68" s="2" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K68" s="4" t="e">
         <f>VLOOKUP(C68,[1]Hoja1!$J:$L,3,0)</f>
@@ -5439,14 +5439,14 @@
       </c>
       <c r="F69" s="3">
         <f t="shared" ca="1" si="15"/>
-        <v>45043</v>
+        <v>45109</v>
       </c>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
       <c r="J69" s="2" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>0 - CCMA - 202304 - 30000000000 - Cliente</v>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="K69" s="4" t="e">
         <f>VLOOKUP(C69,[1]Hoja1!$J:$L,3,0)</f>

</xml_diff>

<commit_message>
Update: Excel Password link formula
</commit_message>
<xml_diff>
--- a/CCMA.xlsx
+++ b/CCMA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\Descarga_CCMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADAE758-D20D-420A-BD13-3A01D9B6A90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA596932-A2A4-4539-B60D-F00643045589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -302,7 +302,7 @@
             <v>20416948926</v>
           </cell>
           <cell r="L11" t="str">
-            <v>Iñakibeitia91</v>
+            <v>Beitia2022</v>
           </cell>
         </row>
         <row r="12">
@@ -324,7 +324,7 @@
             <v>20246008109</v>
           </cell>
           <cell r="L13" t="str">
-            <v>L@rrygrb209</v>
+            <v>L@rrygrb210</v>
           </cell>
         </row>
         <row r="14">
@@ -346,7 +346,7 @@
             <v>30650940667</v>
           </cell>
           <cell r="L15" t="str">
-            <v>Martinb204</v>
+            <v>Martinb202</v>
           </cell>
         </row>
         <row r="16">
@@ -357,7 +357,7 @@
             <v>20147130202</v>
           </cell>
           <cell r="L16" t="str">
-            <v>Martinb204</v>
+            <v>Martinb202</v>
           </cell>
         </row>
         <row r="17">
@@ -368,7 +368,7 @@
             <v>27148268105</v>
           </cell>
           <cell r="L17" t="str">
-            <v>Gracielac275</v>
+            <v>Gracielac276</v>
           </cell>
         </row>
         <row r="18">
@@ -390,7 +390,7 @@
             <v>30707912223</v>
           </cell>
           <cell r="L19" t="str">
-            <v>Gabriela2022</v>
+            <v>Gabriela2023</v>
           </cell>
         </row>
         <row r="20">
@@ -412,7 +412,7 @@
             <v>20303980378</v>
           </cell>
           <cell r="L21" t="str">
-            <v>Sinclair.208</v>
+            <v>Sinclair.209</v>
           </cell>
         </row>
         <row r="22">
@@ -434,7 +434,7 @@
             <v>30672372697</v>
           </cell>
           <cell r="L23" t="str">
-            <v>Carlos2111</v>
+            <v>Carlos1510</v>
           </cell>
         </row>
         <row r="24">
@@ -478,7 +478,7 @@
             <v>27171709925</v>
           </cell>
           <cell r="L27" t="str">
-            <v>Coronasm275</v>
+            <v>Coronasm276</v>
           </cell>
         </row>
         <row r="28">
@@ -500,7 +500,7 @@
             <v>20168291680</v>
           </cell>
           <cell r="L29" t="str">
-            <v>Luisc30001</v>
+            <v>Luisc30002</v>
           </cell>
         </row>
         <row r="30">
@@ -566,7 +566,7 @@
             <v>30709431834</v>
           </cell>
           <cell r="L35" t="str">
-            <v>Marcelo202</v>
+            <v>Marcelo203</v>
           </cell>
         </row>
         <row r="36">
@@ -599,7 +599,7 @@
             <v>20149466356</v>
           </cell>
           <cell r="L38" t="str">
-            <v>REEnriquez207</v>
+            <v>REEnriquez208</v>
           </cell>
         </row>
         <row r="39">
@@ -610,7 +610,7 @@
             <v>20169933031</v>
           </cell>
           <cell r="L39" t="str">
-            <v>Estudio2021</v>
+            <v>Estudio2022</v>
           </cell>
         </row>
         <row r="40">
@@ -621,7 +621,7 @@
             <v>33653520439</v>
           </cell>
           <cell r="L40" t="str">
-            <v>Jcmayol2021</v>
+            <v>Jcmayol2022</v>
           </cell>
         </row>
         <row r="41">
@@ -654,7 +654,7 @@
             <v>20168291834</v>
           </cell>
           <cell r="L43" t="str">
-            <v>TOfi04041965</v>
+            <v>TOfi04041966</v>
           </cell>
         </row>
         <row r="44">
@@ -665,7 +665,7 @@
             <v>20133762761</v>
           </cell>
           <cell r="L44" t="str">
-            <v>Cferreyra59</v>
+            <v>Cferreyra60</v>
           </cell>
         </row>
         <row r="45">
@@ -687,7 +687,7 @@
             <v>23342751644</v>
           </cell>
           <cell r="L46" t="str">
-            <v>VFerreyra89</v>
+            <v>CVFerreyra89</v>
           </cell>
         </row>
         <row r="47">
@@ -698,7 +698,7 @@
             <v>20170394845</v>
           </cell>
           <cell r="L47" t="str">
-            <v>Mferreyra64</v>
+            <v>MJferreyra64</v>
           </cell>
         </row>
         <row r="48">
@@ -764,7 +764,7 @@
             <v>30710404131</v>
           </cell>
           <cell r="L53" t="str">
-            <v>REEnriquez207</v>
+            <v>REEnriquez208</v>
           </cell>
         </row>
         <row r="54">
@@ -802,178 +802,178 @@
         </row>
         <row r="57">
           <cell r="J57">
-            <v>27364071359</v>
+            <v>24056449082</v>
           </cell>
           <cell r="K57">
-            <v>27364071359</v>
+            <v>24056449082</v>
           </cell>
           <cell r="L57" t="str">
-            <v>MelissaH1103</v>
+            <v>Johnny2023</v>
           </cell>
         </row>
         <row r="58">
           <cell r="J58">
-            <v>20149466739</v>
+            <v>27364071359</v>
           </cell>
           <cell r="K58">
-            <v>20149466739</v>
+            <v>27364071359</v>
           </cell>
           <cell r="L58" t="str">
-            <v>Ricardo212</v>
+            <v>MelissaH1104</v>
           </cell>
         </row>
         <row r="59">
           <cell r="J59">
-            <v>20175255819</v>
+            <v>20149466739</v>
           </cell>
           <cell r="K59">
-            <v>33712529909</v>
+            <v>20149466739</v>
           </cell>
           <cell r="L59" t="str">
-            <v>Crispin2022</v>
+            <v>Ricardo212</v>
           </cell>
         </row>
         <row r="60">
           <cell r="J60">
-            <v>20174123072</v>
+            <v>20175255819</v>
           </cell>
           <cell r="K60">
-            <v>20174123072</v>
+            <v>33712529909</v>
           </cell>
           <cell r="L60" t="str">
-            <v>Carlos2111</v>
+            <v>Crispin2022</v>
           </cell>
         </row>
         <row r="61">
           <cell r="J61">
-            <v>20408973598</v>
+            <v>20174123072</v>
           </cell>
           <cell r="K61">
-            <v>20408973598</v>
+            <v>20174123072</v>
           </cell>
           <cell r="L61" t="str">
-            <v>Matiasinsa209</v>
+            <v>Carlos1510</v>
           </cell>
         </row>
         <row r="62">
           <cell r="J62">
-            <v>23377046129</v>
+            <v>20408973598</v>
           </cell>
           <cell r="K62">
-            <v>23377046129</v>
+            <v>20408973598</v>
           </cell>
           <cell r="L62" t="str">
-            <v>Nicolas240</v>
+            <v>Matiasinsa209</v>
           </cell>
         </row>
         <row r="63">
           <cell r="J63">
-            <v>20100325048</v>
+            <v>23377046129</v>
           </cell>
           <cell r="K63">
-            <v>20100325048</v>
+            <v>23377046129</v>
           </cell>
           <cell r="L63" t="str">
-            <v>Jouliae1356</v>
+            <v>Nicolas240</v>
           </cell>
         </row>
         <row r="64">
           <cell r="J64">
-            <v>20175255819</v>
+            <v>20100325048</v>
           </cell>
           <cell r="K64">
-            <v>33712370829</v>
+            <v>20100325048</v>
           </cell>
           <cell r="L64" t="str">
-            <v>Crispin2022</v>
+            <v>Jouliae1356</v>
           </cell>
         </row>
         <row r="65">
           <cell r="J65">
-            <v>27045207388</v>
+            <v>20175255819</v>
           </cell>
           <cell r="K65">
-            <v>27045207388</v>
+            <v>33712370829</v>
           </cell>
           <cell r="L65" t="str">
-            <v>Anamaria2021</v>
+            <v>Crispin2022</v>
           </cell>
         </row>
         <row r="66">
           <cell r="J66">
-            <v>27222731416</v>
+            <v>27045207388</v>
           </cell>
           <cell r="K66">
-            <v>27222731416</v>
+            <v>27045207388</v>
           </cell>
           <cell r="L66" t="str">
-            <v>Nonona2022</v>
+            <v>Anamaria2022</v>
           </cell>
         </row>
         <row r="67">
           <cell r="J67">
-            <v>27058846916</v>
+            <v>27222731416</v>
           </cell>
           <cell r="K67">
-            <v>27058846916</v>
+            <v>27222731416</v>
           </cell>
           <cell r="L67" t="str">
-            <v>Lazcozh277</v>
+            <v>Nonona2022</v>
           </cell>
         </row>
         <row r="68">
           <cell r="J68">
-            <v>23385665709</v>
+            <v>27058846916</v>
           </cell>
           <cell r="K68">
-            <v>23385665709</v>
+            <v>27058846916</v>
           </cell>
           <cell r="L68" t="str">
-            <v>Dallas5058</v>
+            <v>Lazcozh277</v>
           </cell>
         </row>
         <row r="69">
           <cell r="J69">
-            <v>23120538209</v>
+            <v>23385665709</v>
           </cell>
           <cell r="K69">
-            <v>23120538209</v>
+            <v>23385665709</v>
           </cell>
           <cell r="L69" t="str">
-            <v>Pliniolin239</v>
+            <v>Dallas5058</v>
           </cell>
         </row>
         <row r="70">
           <cell r="J70">
-            <v>27173878309</v>
+            <v>23120538209</v>
           </cell>
           <cell r="K70">
-            <v>27173878309</v>
+            <v>23120538209</v>
           </cell>
           <cell r="L70" t="str">
-            <v>Lionettoc280</v>
+            <v>Pliniolin240</v>
           </cell>
         </row>
         <row r="71">
           <cell r="J71">
-            <v>20203385049</v>
+            <v>27173878309</v>
           </cell>
           <cell r="K71">
-            <v>20203385049</v>
+            <v>27173878309</v>
           </cell>
           <cell r="L71" t="str">
-            <v>Posadas4601</v>
+            <v>Lionettoc280</v>
           </cell>
         </row>
         <row r="72">
           <cell r="J72">
-            <v>23173121539</v>
+            <v>20203385049</v>
           </cell>
           <cell r="K72">
-            <v>23173121539</v>
+            <v>20203385049</v>
           </cell>
           <cell r="L72" t="str">
-            <v>Posadas4602</v>
+            <v>Posadas4601</v>
           </cell>
         </row>
         <row r="73">
@@ -989,541 +989,563 @@
         </row>
         <row r="74">
           <cell r="J74">
-            <v>23246015139</v>
+            <v>23173121539</v>
           </cell>
           <cell r="K74">
-            <v>23246015139</v>
+            <v>23173121539</v>
           </cell>
           <cell r="L74" t="str">
-            <v>Posadas4919</v>
+            <v>Posadas4602</v>
           </cell>
         </row>
         <row r="75">
           <cell r="J75">
-            <v>27163651918</v>
+            <v>23246015139</v>
           </cell>
           <cell r="K75">
-            <v>27163651918</v>
+            <v>23246015139</v>
           </cell>
           <cell r="L75" t="str">
-            <v>Martina2783</v>
+            <v>Posadas4919</v>
           </cell>
         </row>
         <row r="76">
           <cell r="J76">
-            <v>20168296011</v>
+            <v>27163651918</v>
           </cell>
           <cell r="K76">
-            <v>20168296011</v>
+            <v>27163651918</v>
           </cell>
           <cell r="L76" t="str">
-            <v>Jcmayol2021</v>
+            <v>Martina2783</v>
           </cell>
         </row>
         <row r="77">
           <cell r="J77">
-            <v>20203383666</v>
+            <v>20168296011</v>
           </cell>
           <cell r="K77">
-            <v>20203383666</v>
+            <v>20168296011</v>
           </cell>
           <cell r="L77" t="str">
-            <v>Rmayol2021</v>
+            <v>Jcmayol2022</v>
           </cell>
         </row>
         <row r="78">
           <cell r="J78">
-            <v>20133762761</v>
+            <v>20203383666</v>
           </cell>
           <cell r="K78">
-            <v>30657146850</v>
+            <v>20203383666</v>
           </cell>
           <cell r="L78" t="str">
-            <v>Cferreyra59</v>
+            <v>Rmayol2022</v>
           </cell>
         </row>
         <row r="79">
           <cell r="J79">
-            <v>27128520851</v>
+            <v>20133762761</v>
           </cell>
           <cell r="K79">
-            <v>27128520851</v>
+            <v>30657146850</v>
           </cell>
           <cell r="L79" t="str">
-            <v>Molaspatricia272</v>
+            <v>Cferreyra60</v>
           </cell>
         </row>
         <row r="80">
           <cell r="J80">
-            <v>20077065637</v>
+            <v>27128520851</v>
           </cell>
           <cell r="K80">
-            <v>20077065637</v>
+            <v>27128520851</v>
           </cell>
           <cell r="L80" t="str">
-            <v>PEnsaanibal207</v>
+            <v>Molaspatricia273</v>
           </cell>
         </row>
         <row r="81">
           <cell r="J81">
-            <v>20343667966</v>
+            <v>20077065637</v>
           </cell>
           <cell r="K81">
-            <v>20343667966</v>
+            <v>20077065637</v>
           </cell>
           <cell r="L81" t="str">
-            <v>bruno206</v>
+            <v>PEnsaanibal208</v>
           </cell>
         </row>
         <row r="82">
           <cell r="J82">
-            <v>20075878495</v>
+            <v>20343667966</v>
           </cell>
           <cell r="K82">
-            <v>20075878495</v>
+            <v>20343667966</v>
           </cell>
           <cell r="L82" t="str">
-            <v>Roberto205</v>
+            <v>bruno206</v>
           </cell>
         </row>
         <row r="83">
           <cell r="J83">
-            <v>20334250327</v>
+            <v>20075878495</v>
           </cell>
           <cell r="K83">
-            <v>20334250327</v>
+            <v>20075878495</v>
           </cell>
           <cell r="L83" t="str">
-            <v>Pensalu208</v>
+            <v>Roberto205</v>
           </cell>
         </row>
         <row r="84">
           <cell r="J84">
-            <v>27354872183</v>
+            <v>20334250327</v>
           </cell>
           <cell r="K84">
-            <v>27354872183</v>
+            <v>20334250327</v>
           </cell>
           <cell r="L84" t="str">
-            <v>Peugenia273</v>
+            <v>Pensalu208</v>
           </cell>
         </row>
         <row r="85">
           <cell r="J85">
-            <v>20085452291</v>
+            <v>27354872183</v>
           </cell>
           <cell r="K85">
-            <v>20085452291</v>
+            <v>27354872183</v>
           </cell>
           <cell r="L85" t="str">
-            <v>Oscarp2022</v>
+            <v>Peugenia275</v>
           </cell>
         </row>
         <row r="86">
           <cell r="J86">
-            <v>20334250327</v>
+            <v>20085452291</v>
           </cell>
           <cell r="K86">
-            <v>30716503816</v>
+            <v>20085452291</v>
           </cell>
           <cell r="L86" t="str">
-            <v>Pensalu208</v>
+            <v>Oscarp2022</v>
           </cell>
         </row>
         <row r="87">
           <cell r="J87">
-            <v>27176756751</v>
-          </cell>
-          <cell r="K87" t="e">
-            <v>#VALUE!</v>
+            <v>20334250327</v>
+          </cell>
+          <cell r="K87">
+            <v>30716503816</v>
           </cell>
           <cell r="L87" t="str">
-            <v>aTHENUCHI06</v>
+            <v>Pensalu208</v>
           </cell>
         </row>
         <row r="88">
           <cell r="J88">
-            <v>20172521771</v>
-          </cell>
-          <cell r="K88">
-            <v>20172521771</v>
+            <v>27176756751</v>
+          </cell>
+          <cell r="K88" t="e">
+            <v>#VALUE!</v>
           </cell>
           <cell r="L88" t="str">
-            <v>Pereyra2022</v>
+            <v>aTHENUCHI06</v>
           </cell>
         </row>
         <row r="89">
           <cell r="J89">
-            <v>20115533003</v>
+            <v>20172521771</v>
           </cell>
           <cell r="K89">
-            <v>20115533003</v>
+            <v>20172521771</v>
           </cell>
           <cell r="L89" t="str">
-            <v>Jorgefer2021</v>
+            <v>Pereyra2022</v>
           </cell>
         </row>
         <row r="90">
           <cell r="J90">
-            <v>27169311027</v>
+            <v>20115533003</v>
           </cell>
           <cell r="K90">
-            <v>27169311027</v>
+            <v>20115533003</v>
           </cell>
           <cell r="L90" t="str">
-            <v>Piasentinia277</v>
+            <v>Jorgefer2021</v>
           </cell>
         </row>
         <row r="91">
           <cell r="J91">
-            <v>27176756751</v>
+            <v>27169311027</v>
           </cell>
           <cell r="K91">
-            <v>27176756751</v>
+            <v>27169311027</v>
           </cell>
           <cell r="L91" t="str">
-            <v>aTHENUCHI06</v>
+            <v>Piasentinia277</v>
           </cell>
         </row>
         <row r="92">
           <cell r="J92">
-            <v>20100325048</v>
+            <v>27176756751</v>
           </cell>
           <cell r="K92">
-            <v>30708370122</v>
+            <v>27176756751</v>
           </cell>
           <cell r="L92" t="str">
-            <v>Jouliae1356</v>
+            <v>aTHENUCHI06</v>
           </cell>
         </row>
         <row r="93">
           <cell r="J93">
-            <v>20109908852</v>
+            <v>20100325048</v>
           </cell>
           <cell r="K93">
-            <v>30687910636</v>
+            <v>30708370122</v>
           </cell>
           <cell r="L93" t="str">
-            <v>Robertob2330</v>
+            <v>Jouliae1356</v>
           </cell>
         </row>
         <row r="94">
           <cell r="J94">
-            <v>20168291931</v>
+            <v>20109908852</v>
           </cell>
           <cell r="K94">
-            <v>30709206695</v>
+            <v>30687910636</v>
           </cell>
           <cell r="L94" t="str">
-            <v>apipeAPIPE789</v>
+            <v>RobertoB2330</v>
           </cell>
         </row>
         <row r="95">
           <cell r="J95">
-            <v>20309592159</v>
+            <v>20168291931</v>
           </cell>
           <cell r="K95">
-            <v>20309592159</v>
+            <v>30709206695</v>
           </cell>
           <cell r="L95" t="str">
-            <v>Rieraariel209</v>
+            <v>apipeAPIPE789</v>
           </cell>
         </row>
         <row r="96">
           <cell r="J96">
-            <v>20121182832</v>
+            <v>20309592159</v>
           </cell>
           <cell r="K96">
-            <v>20121182832</v>
+            <v>20309592159</v>
           </cell>
           <cell r="L96" t="str">
-            <v>RieraManuel202</v>
+            <v>Rieraariel209</v>
           </cell>
         </row>
         <row r="97">
           <cell r="J97">
-            <v>20173120282</v>
+            <v>20121182832</v>
           </cell>
           <cell r="K97">
-            <v>20173120282</v>
+            <v>20121182832</v>
           </cell>
           <cell r="L97" t="str">
-            <v>Marcelo2021</v>
+            <v>RieraManuel2023</v>
           </cell>
         </row>
         <row r="98">
           <cell r="J98">
-            <v>27217236547</v>
+            <v>20173120282</v>
           </cell>
           <cell r="K98">
-            <v>27217236547</v>
+            <v>20173120282</v>
           </cell>
           <cell r="L98" t="str">
-            <v>Florencia2000</v>
+            <v>Marcelo2021</v>
           </cell>
         </row>
         <row r="99">
           <cell r="J99">
-            <v>20116452023</v>
+            <v>27217236547</v>
           </cell>
           <cell r="K99">
-            <v>30510926583</v>
+            <v>27217236547</v>
           </cell>
           <cell r="L99" t="str">
-            <v>Ljrc421992</v>
+            <v>Florencia2000</v>
           </cell>
         </row>
         <row r="100">
           <cell r="J100">
-            <v>23351897074</v>
+            <v>20116452023</v>
           </cell>
           <cell r="K100">
-            <v>23351897074</v>
+            <v>30510926583</v>
           </cell>
           <cell r="L100" t="str">
-            <v>Lucila2022</v>
+            <v>Ljrc421992</v>
           </cell>
         </row>
         <row r="101">
           <cell r="J101">
-            <v>27109797257</v>
+            <v>23351897074</v>
           </cell>
           <cell r="K101">
-            <v>27109797257</v>
+            <v>23351897074</v>
           </cell>
           <cell r="L101" t="str">
-            <v>Olgascotto279</v>
+            <v>Lucila2022</v>
           </cell>
         </row>
         <row r="102">
           <cell r="J102">
-            <v>27068286323</v>
+            <v>27109797257</v>
           </cell>
           <cell r="K102">
-            <v>27068286323</v>
+            <v>27109797257</v>
           </cell>
           <cell r="L102" t="str">
-            <v>Sesmero2022</v>
+            <v>Olgascotto279</v>
           </cell>
         </row>
         <row r="103">
           <cell r="J103">
-            <v>27067089680</v>
+            <v>27068286323</v>
           </cell>
           <cell r="K103">
-            <v>27067089680</v>
+            <v>27068286323</v>
           </cell>
           <cell r="L103" t="str">
-            <v>Tsesmero271</v>
+            <v>Sesmero2023</v>
           </cell>
         </row>
         <row r="104">
           <cell r="J104">
-            <v>23149462074</v>
+            <v>27067089680</v>
           </cell>
           <cell r="K104">
-            <v>23149462074</v>
+            <v>27067089680</v>
           </cell>
           <cell r="L104" t="str">
-            <v>Gabriela2022</v>
+            <v>Tsesmero272</v>
           </cell>
         </row>
         <row r="105">
           <cell r="J105">
-            <v>23248265159</v>
+            <v>23149462074</v>
           </cell>
           <cell r="K105">
-            <v>23248265159</v>
+            <v>23149462074</v>
           </cell>
           <cell r="L105" t="str">
-            <v>Sebastian10</v>
+            <v>Gabriela2023</v>
           </cell>
         </row>
         <row r="106">
           <cell r="J106">
-            <v>23242946669</v>
+            <v>23248265159</v>
           </cell>
           <cell r="K106">
-            <v>23242946669</v>
+            <v>23248265159</v>
           </cell>
           <cell r="L106" t="str">
-            <v>Miguelsoto666</v>
+            <v>Sebastian10</v>
           </cell>
         </row>
         <row r="107">
           <cell r="J107">
-            <v>27201932268</v>
+            <v>23242946669</v>
           </cell>
           <cell r="K107">
-            <v>27201932268</v>
+            <v>23242946669</v>
           </cell>
           <cell r="L107" t="str">
-            <v>Samanta1035</v>
+            <v>Miguelsoto667</v>
           </cell>
         </row>
         <row r="108">
           <cell r="J108">
-            <v>27201178776</v>
+            <v>27201932268</v>
           </cell>
           <cell r="K108">
-            <v>27201178776</v>
+            <v>27201932268</v>
           </cell>
           <cell r="L108" t="str">
-            <v>Monicaszy22</v>
+            <v>Samanta1035</v>
           </cell>
         </row>
         <row r="109">
           <cell r="J109">
-            <v>27348916942</v>
+            <v>27201178776</v>
           </cell>
           <cell r="K109">
-            <v>27348916942</v>
+            <v>27201178776</v>
           </cell>
           <cell r="L109" t="str">
-            <v>karen580</v>
+            <v>Monicaszy11</v>
           </cell>
         </row>
         <row r="110">
           <cell r="J110">
-            <v>20149462601</v>
+            <v>27348916942</v>
           </cell>
           <cell r="K110">
-            <v>20149462601</v>
+            <v>27348916942</v>
           </cell>
           <cell r="L110" t="str">
-            <v>Marcelo202</v>
+            <v>karen580</v>
           </cell>
         </row>
         <row r="111">
           <cell r="J111">
-            <v>20074827455</v>
+            <v>20149462601</v>
           </cell>
           <cell r="K111">
-            <v>20074827455</v>
+            <v>20149462601</v>
           </cell>
           <cell r="L111" t="str">
-            <v>Ricardo102</v>
+            <v>Marcelo203</v>
           </cell>
         </row>
         <row r="112">
           <cell r="J112">
-            <v>20130056637</v>
+            <v>20074827455</v>
           </cell>
           <cell r="K112">
-            <v>20130056637</v>
+            <v>20074827455</v>
           </cell>
           <cell r="L112" t="str">
-            <v>Tabbiae207</v>
+            <v>Ricardo103</v>
           </cell>
         </row>
         <row r="113">
           <cell r="J113">
-            <v>20133762761</v>
+            <v>20130056637</v>
           </cell>
           <cell r="K113">
-            <v>30715577743</v>
+            <v>20130056637</v>
           </cell>
           <cell r="L113" t="str">
-            <v>Cferreyra59</v>
+            <v>Tabbiae208</v>
           </cell>
         </row>
         <row r="114">
           <cell r="J114">
-            <v>27236873744</v>
+            <v>20133762761</v>
           </cell>
           <cell r="K114">
-            <v>27236873744</v>
+            <v>30715577743</v>
           </cell>
           <cell r="L114" t="str">
-            <v>Sotomalena0818</v>
+            <v>Cferreyra60</v>
           </cell>
         </row>
         <row r="115">
           <cell r="J115">
-            <v>20051985967</v>
+            <v>27236873744</v>
           </cell>
           <cell r="K115">
-            <v>20051985967</v>
+            <v>27236873744</v>
           </cell>
           <cell r="L115" t="str">
-            <v>Andres5967</v>
+            <v>Sotomalena0818</v>
           </cell>
         </row>
         <row r="116">
           <cell r="J116">
-            <v>20230966738</v>
+            <v>20051985967</v>
           </cell>
           <cell r="K116">
-            <v>20230966738</v>
+            <v>20051985967</v>
           </cell>
           <cell r="L116" t="str">
-            <v>Durrutia4440</v>
+            <v>Andres5967</v>
           </cell>
         </row>
         <row r="117">
           <cell r="J117">
-            <v>27116976620</v>
+            <v>20230966738</v>
           </cell>
           <cell r="K117">
-            <v>27116976620</v>
+            <v>20230966738</v>
           </cell>
           <cell r="L117" t="str">
-            <v>Miriamu272</v>
+            <v>Durrutia4441</v>
           </cell>
         </row>
         <row r="118">
           <cell r="J118">
-            <v>20044483441</v>
-          </cell>
-          <cell r="K118" t="e">
-            <v>#VALUE!</v>
+            <v>27116976620</v>
+          </cell>
+          <cell r="K118">
+            <v>27116976620</v>
           </cell>
           <cell r="L118" t="str">
-            <v>Calafate2022</v>
+            <v>Miriamu272</v>
           </cell>
         </row>
         <row r="119">
           <cell r="J119">
-            <v>20315731330</v>
-          </cell>
-          <cell r="K119">
-            <v>20315731330</v>
+            <v>20044483441</v>
+          </cell>
+          <cell r="K119" t="e">
+            <v>#VALUE!</v>
           </cell>
           <cell r="L119" t="str">
-            <v>AngelGV200</v>
+            <v>Calafate2022</v>
           </cell>
         </row>
         <row r="120">
           <cell r="J120">
-            <v>20110780525</v>
+            <v>20315731330</v>
           </cell>
           <cell r="K120">
-            <v>20110780525</v>
+            <v>20315731330</v>
           </cell>
           <cell r="L120" t="str">
-            <v>vare205</v>
+            <v>AngelGV200</v>
           </cell>
         </row>
         <row r="121">
           <cell r="J121">
-            <v>20301650087</v>
+            <v>20110780525</v>
           </cell>
           <cell r="K121">
-            <v>20301650087</v>
+            <v>20110780525</v>
           </cell>
           <cell r="L121" t="str">
-            <v>VarenizaLeo208</v>
+            <v>vare205</v>
           </cell>
         </row>
         <row r="122">
           <cell r="J122">
+            <v>20301650087</v>
+          </cell>
+          <cell r="K122">
+            <v>20301650087</v>
+          </cell>
+          <cell r="L122" t="str">
+            <v>VarenizaLeo208</v>
+          </cell>
+        </row>
+        <row r="123">
+          <cell r="J123">
             <v>20334250327</v>
           </cell>
-          <cell r="K122">
+          <cell r="K123">
             <v>30715795864</v>
           </cell>
-          <cell r="L122" t="str">
+          <cell r="L123" t="str">
             <v>Pensalu208</v>
+          </cell>
+        </row>
+        <row r="124">
+          <cell r="J124">
+            <v>27142090959</v>
+          </cell>
+          <cell r="K124">
+            <v>27142090959</v>
+          </cell>
+          <cell r="L124" t="str">
+            <v>Trapito5058</v>
           </cell>
         </row>
       </sheetData>
@@ -1800,7 +1822,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1887,7 +1909,7 @@
       </c>
       <c r="F2" s="3">
         <f ca="1">TODAY()</f>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -1896,13 +1918,13 @@
         <f ca="1">CONCATENATE(TEXT(A2,"0")," - ","CCMA - ",YEAR(F2)&amp;TEXT(MONTH(F2),"00")," - ",SUBSTITUTE(D2,"-","")," - ",B2)</f>
         <v>0 - CCMA - 202307 - 20000000000 - Cliente</v>
       </c>
-      <c r="K2" s="4" t="e">
-        <f>VLOOKUP(C2,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L2" s="5" t="e">
+      <c r="K2" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C2,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L2" s="5" t="str">
         <f t="shared" ref="L2:L33" si="1">IF(EXACT(K2,E2),"ü","x")</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M2" s="4">
         <f t="shared" ref="M2:M33" si="2">ROW(A2)</f>
@@ -1941,7 +1963,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F66" ca="1" si="6">TODAY()</f>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1950,13 +1972,13 @@
         <f t="shared" ref="J3:J66" ca="1" si="7">CONCATENATE(TEXT(A3,"0")," - ","CCMA - ",YEAR(F3)&amp;TEXT(MONTH(F3),"00")," - ",SUBSTITUTE(D3,"-","")," - ",B3)</f>
         <v>0 - CCMA - 202307 - 20000000000 - Cliente</v>
       </c>
-      <c r="K3" s="4" t="e">
-        <f>VLOOKUP(C3,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L3" s="5" t="e">
+      <c r="K3" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C3,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L3" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M3" s="4">
         <f t="shared" si="2"/>
@@ -1994,7 +2016,7 @@
       </c>
       <c r="F4" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -2003,13 +2025,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K4" s="4" t="e">
-        <f>VLOOKUP(C4,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L4" s="5" t="e">
+      <c r="K4" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C4,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L4" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M4" s="4">
         <f t="shared" si="2"/>
@@ -2047,7 +2069,7 @@
       </c>
       <c r="F5" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -2056,13 +2078,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K5" s="4" t="e">
-        <f>VLOOKUP(C5,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L5" s="5" t="e">
+      <c r="K5" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C5,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L5" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M5" s="4">
         <f t="shared" si="2"/>
@@ -2100,7 +2122,7 @@
       </c>
       <c r="F6" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -2109,13 +2131,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K6" s="4" t="e">
-        <f>VLOOKUP(C6,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L6" s="5" t="e">
+      <c r="K6" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C6,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L6" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M6" s="4">
         <f t="shared" si="2"/>
@@ -2153,7 +2175,7 @@
       </c>
       <c r="F7" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -2162,13 +2184,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K7" s="4" t="e">
-        <f>VLOOKUP(C7,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L7" s="5" t="e">
+      <c r="K7" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C7,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L7" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M7" s="4">
         <f t="shared" si="2"/>
@@ -2206,7 +2228,7 @@
       </c>
       <c r="F8" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -2215,13 +2237,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K8" s="4" t="e">
-        <f>VLOOKUP(C8,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L8" s="5" t="e">
+      <c r="K8" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C8,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L8" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M8" s="4">
         <f t="shared" si="2"/>
@@ -2259,7 +2281,7 @@
       </c>
       <c r="F9" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -2268,13 +2290,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K9" s="4" t="e">
-        <f>VLOOKUP(C9,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L9" s="5" t="e">
+      <c r="K9" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C9,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L9" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M9" s="4">
         <f t="shared" si="2"/>
@@ -2312,7 +2334,7 @@
       </c>
       <c r="F10" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -2321,13 +2343,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K10" s="4" t="e">
-        <f>VLOOKUP(C10,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L10" s="5" t="e">
+      <c r="K10" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C10,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L10" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M10" s="4">
         <f t="shared" si="2"/>
@@ -2365,7 +2387,7 @@
       </c>
       <c r="F11" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -2374,13 +2396,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K11" s="4" t="e">
-        <f>VLOOKUP(C11,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L11" s="5" t="e">
+      <c r="K11" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C11,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L11" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M11" s="4">
         <f t="shared" si="2"/>
@@ -2418,7 +2440,7 @@
       </c>
       <c r="F12" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -2427,13 +2449,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K12" s="4" t="e">
-        <f>VLOOKUP(C12,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L12" s="5" t="e">
+      <c r="K12" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C12,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L12" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M12" s="4">
         <f t="shared" si="2"/>
@@ -2471,7 +2493,7 @@
       </c>
       <c r="F13" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -2480,13 +2502,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K13" s="4" t="e">
-        <f>VLOOKUP(C13,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L13" s="5" t="e">
+      <c r="K13" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C13,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L13" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M13" s="4">
         <f t="shared" si="2"/>
@@ -2524,7 +2546,7 @@
       </c>
       <c r="F14" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -2533,13 +2555,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K14" s="4" t="e">
-        <f>VLOOKUP(C14,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L14" s="5" t="e">
+      <c r="K14" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C14,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L14" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M14" s="4">
         <f t="shared" si="2"/>
@@ -2577,7 +2599,7 @@
       </c>
       <c r="F15" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -2586,13 +2608,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K15" s="4" t="e">
-        <f>VLOOKUP(C15,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L15" s="5" t="e">
+      <c r="K15" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C15,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L15" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M15" s="4">
         <f t="shared" si="2"/>
@@ -2630,7 +2652,7 @@
       </c>
       <c r="F16" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -2639,13 +2661,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K16" s="4" t="e">
-        <f>VLOOKUP(C16,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L16" s="5" t="e">
+      <c r="K16" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C16,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L16" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M16" s="4">
         <f t="shared" si="2"/>
@@ -2683,7 +2705,7 @@
       </c>
       <c r="F17" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -2692,13 +2714,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K17" s="4" t="e">
-        <f>VLOOKUP(C17,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L17" s="5" t="e">
+      <c r="K17" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C17,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L17" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M17" s="4">
         <f t="shared" si="2"/>
@@ -2736,7 +2758,7 @@
       </c>
       <c r="F18" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -2745,13 +2767,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K18" s="4" t="e">
-        <f>VLOOKUP(C18,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L18" s="5" t="e">
+      <c r="K18" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C18,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L18" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M18" s="4">
         <f t="shared" si="2"/>
@@ -2789,7 +2811,7 @@
       </c>
       <c r="F19" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -2798,13 +2820,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K19" s="4" t="e">
-        <f>VLOOKUP(C19,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L19" s="5" t="e">
+      <c r="K19" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C19,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L19" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M19" s="4">
         <f t="shared" si="2"/>
@@ -2842,7 +2864,7 @@
       </c>
       <c r="F20" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -2851,13 +2873,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K20" s="4" t="e">
-        <f>VLOOKUP(C20,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L20" s="5" t="e">
+      <c r="K20" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C20,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L20" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M20" s="4">
         <f t="shared" si="2"/>
@@ -2895,7 +2917,7 @@
       </c>
       <c r="F21" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -2904,13 +2926,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K21" s="4" t="e">
-        <f>VLOOKUP(C21,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L21" s="5" t="e">
+      <c r="K21" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C21,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L21" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M21" s="4">
         <f t="shared" si="2"/>
@@ -2948,7 +2970,7 @@
       </c>
       <c r="F22" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -2957,13 +2979,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K22" s="4" t="e">
-        <f>VLOOKUP(C22,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L22" s="5" t="e">
+      <c r="K22" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C22,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L22" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M22" s="4">
         <f t="shared" si="2"/>
@@ -3001,7 +3023,7 @@
       </c>
       <c r="F23" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -3010,13 +3032,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K23" s="4" t="e">
-        <f>VLOOKUP(C23,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L23" s="5" t="e">
+      <c r="K23" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C23,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L23" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M23" s="4">
         <f t="shared" si="2"/>
@@ -3054,7 +3076,7 @@
       </c>
       <c r="F24" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -3063,13 +3085,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K24" s="4" t="e">
-        <f>VLOOKUP(C24,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L24" s="5" t="e">
+      <c r="K24" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C24,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L24" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M24" s="4">
         <f t="shared" si="2"/>
@@ -3107,7 +3129,7 @@
       </c>
       <c r="F25" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -3116,13 +3138,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K25" s="4" t="e">
-        <f>VLOOKUP(C25,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L25" s="5" t="e">
+      <c r="K25" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C25,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L25" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M25" s="4">
         <f t="shared" si="2"/>
@@ -3160,7 +3182,7 @@
       </c>
       <c r="F26" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -3169,13 +3191,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K26" s="4" t="e">
-        <f>VLOOKUP(C26,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L26" s="5" t="e">
+      <c r="K26" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C26,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L26" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M26" s="4">
         <f t="shared" si="2"/>
@@ -3213,7 +3235,7 @@
       </c>
       <c r="F27" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -3222,13 +3244,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K27" s="4" t="e">
-        <f>VLOOKUP(C27,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L27" s="5" t="e">
+      <c r="K27" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C27,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L27" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M27" s="4">
         <f t="shared" si="2"/>
@@ -3266,7 +3288,7 @@
       </c>
       <c r="F28" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -3275,13 +3297,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K28" s="4" t="e">
-        <f>VLOOKUP(C28,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L28" s="5" t="e">
+      <c r="K28" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C28,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L28" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M28" s="4">
         <f t="shared" si="2"/>
@@ -3319,7 +3341,7 @@
       </c>
       <c r="F29" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -3328,13 +3350,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K29" s="4" t="e">
-        <f>VLOOKUP(C29,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L29" s="5" t="e">
+      <c r="K29" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C29,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L29" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M29" s="4">
         <f t="shared" si="2"/>
@@ -3372,7 +3394,7 @@
       </c>
       <c r="F30" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -3381,13 +3403,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K30" s="4" t="e">
-        <f>VLOOKUP(C30,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L30" s="5" t="e">
+      <c r="K30" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C30,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L30" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M30" s="4">
         <f t="shared" si="2"/>
@@ -3425,7 +3447,7 @@
       </c>
       <c r="F31" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -3434,13 +3456,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K31" s="4" t="e">
-        <f>VLOOKUP(C31,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L31" s="5" t="e">
+      <c r="K31" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C31,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L31" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M31" s="4">
         <f t="shared" si="2"/>
@@ -3478,7 +3500,7 @@
       </c>
       <c r="F32" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -3487,13 +3509,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K32" s="4" t="e">
-        <f>VLOOKUP(C32,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L32" s="5" t="e">
+      <c r="K32" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C32,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L32" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M32" s="4">
         <f t="shared" si="2"/>
@@ -3531,7 +3553,7 @@
       </c>
       <c r="F33" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -3540,13 +3562,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K33" s="4" t="e">
-        <f>VLOOKUP(C33,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L33" s="5" t="e">
+      <c r="K33" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C33,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L33" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M33" s="4">
         <f t="shared" si="2"/>
@@ -3584,7 +3606,7 @@
       </c>
       <c r="F34" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -3593,13 +3615,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K34" s="4" t="e">
-        <f>VLOOKUP(C34,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L34" s="5" t="e">
+      <c r="K34" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C34,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L34" s="5" t="str">
         <f t="shared" ref="L34:L65" si="12">IF(EXACT(K34,E34),"ü","x")</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M34" s="4">
         <f t="shared" ref="M34:M69" si="13">ROW(A34)</f>
@@ -3637,7 +3659,7 @@
       </c>
       <c r="F35" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -3646,13 +3668,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K35" s="4" t="e">
-        <f>VLOOKUP(C35,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L35" s="5" t="e">
+      <c r="K35" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C35,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L35" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M35" s="4">
         <f t="shared" si="13"/>
@@ -3690,7 +3712,7 @@
       </c>
       <c r="F36" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -3699,13 +3721,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K36" s="4" t="e">
-        <f>VLOOKUP(C36,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L36" s="5" t="e">
+      <c r="K36" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C36,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L36" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M36" s="4">
         <f t="shared" si="13"/>
@@ -3743,7 +3765,7 @@
       </c>
       <c r="F37" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -3752,13 +3774,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K37" s="4" t="e">
-        <f>VLOOKUP(C37,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L37" s="5" t="e">
+      <c r="K37" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C37,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L37" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M37" s="4">
         <f t="shared" si="13"/>
@@ -3796,7 +3818,7 @@
       </c>
       <c r="F38" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -3805,13 +3827,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K38" s="4" t="e">
-        <f>VLOOKUP(C38,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L38" s="5" t="e">
+      <c r="K38" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C38,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L38" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M38" s="4">
         <f t="shared" si="13"/>
@@ -3849,7 +3871,7 @@
       </c>
       <c r="F39" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -3858,13 +3880,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K39" s="4" t="e">
-        <f>VLOOKUP(C39,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L39" s="5" t="e">
+      <c r="K39" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C39,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L39" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M39" s="4">
         <f t="shared" si="13"/>
@@ -3902,7 +3924,7 @@
       </c>
       <c r="F40" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
@@ -3911,13 +3933,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K40" s="4" t="e">
-        <f>VLOOKUP(C40,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L40" s="5" t="e">
+      <c r="K40" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C40,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L40" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M40" s="4">
         <f t="shared" si="13"/>
@@ -3955,7 +3977,7 @@
       </c>
       <c r="F41" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -3964,13 +3986,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K41" s="4" t="e">
-        <f>VLOOKUP(C41,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L41" s="5" t="e">
+      <c r="K41" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C41,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L41" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M41" s="4">
         <f t="shared" si="13"/>
@@ -4008,7 +4030,7 @@
       </c>
       <c r="F42" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -4017,13 +4039,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K42" s="4" t="e">
-        <f>VLOOKUP(C42,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L42" s="5" t="e">
+      <c r="K42" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C42,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L42" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M42" s="4">
         <f t="shared" si="13"/>
@@ -4061,7 +4083,7 @@
       </c>
       <c r="F43" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -4070,13 +4092,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K43" s="4" t="e">
-        <f>VLOOKUP(C43,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L43" s="5" t="e">
+      <c r="K43" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C43,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L43" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M43" s="4">
         <f t="shared" si="13"/>
@@ -4114,7 +4136,7 @@
       </c>
       <c r="F44" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -4123,13 +4145,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K44" s="4" t="e">
-        <f>VLOOKUP(C44,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L44" s="5" t="e">
+      <c r="K44" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C44,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L44" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M44" s="4">
         <f t="shared" si="13"/>
@@ -4167,7 +4189,7 @@
       </c>
       <c r="F45" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -4176,13 +4198,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K45" s="4" t="e">
-        <f>VLOOKUP(C45,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L45" s="5" t="e">
+      <c r="K45" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C45,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L45" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M45" s="4">
         <f t="shared" si="13"/>
@@ -4220,7 +4242,7 @@
       </c>
       <c r="F46" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -4229,13 +4251,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K46" s="4" t="e">
-        <f>VLOOKUP(C46,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L46" s="5" t="e">
+      <c r="K46" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C46,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L46" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M46" s="4">
         <f t="shared" si="13"/>
@@ -4273,7 +4295,7 @@
       </c>
       <c r="F47" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -4282,13 +4304,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K47" s="4" t="e">
-        <f>VLOOKUP(C47,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L47" s="5" t="e">
+      <c r="K47" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C47,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L47" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M47" s="4">
         <f t="shared" si="13"/>
@@ -4326,7 +4348,7 @@
       </c>
       <c r="F48" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
@@ -4335,13 +4357,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K48" s="4" t="e">
-        <f>VLOOKUP(C48,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L48" s="5" t="e">
+      <c r="K48" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C48,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L48" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M48" s="4">
         <f t="shared" si="13"/>
@@ -4379,7 +4401,7 @@
       </c>
       <c r="F49" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
@@ -4388,13 +4410,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K49" s="4" t="e">
-        <f>VLOOKUP(C49,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L49" s="5" t="e">
+      <c r="K49" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C49,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L49" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M49" s="4">
         <f t="shared" si="13"/>
@@ -4432,7 +4454,7 @@
       </c>
       <c r="F50" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -4441,13 +4463,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K50" s="4" t="e">
-        <f>VLOOKUP(C50,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L50" s="5" t="e">
+      <c r="K50" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C50,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L50" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M50" s="4">
         <f t="shared" si="13"/>
@@ -4485,7 +4507,7 @@
       </c>
       <c r="F51" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -4494,13 +4516,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K51" s="4" t="e">
-        <f>VLOOKUP(C51,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L51" s="5" t="e">
+      <c r="K51" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C51,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L51" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M51" s="4">
         <f t="shared" si="13"/>
@@ -4538,7 +4560,7 @@
       </c>
       <c r="F52" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -4547,13 +4569,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K52" s="4" t="e">
-        <f>VLOOKUP(C52,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L52" s="5" t="e">
+      <c r="K52" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C52,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L52" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M52" s="4">
         <f t="shared" si="13"/>
@@ -4591,7 +4613,7 @@
       </c>
       <c r="F53" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
@@ -4600,13 +4622,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K53" s="4" t="e">
-        <f>VLOOKUP(C53,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L53" s="5" t="e">
+      <c r="K53" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C53,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L53" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M53" s="4">
         <f t="shared" si="13"/>
@@ -4644,7 +4666,7 @@
       </c>
       <c r="F54" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
@@ -4653,13 +4675,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K54" s="4" t="e">
-        <f>VLOOKUP(C54,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L54" s="5" t="e">
+      <c r="K54" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C54,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L54" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M54" s="4">
         <f t="shared" si="13"/>
@@ -4697,7 +4719,7 @@
       </c>
       <c r="F55" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
@@ -4706,13 +4728,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K55" s="4" t="e">
-        <f>VLOOKUP(C55,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L55" s="5" t="e">
+      <c r="K55" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C55,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L55" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M55" s="4">
         <f t="shared" si="13"/>
@@ -4750,7 +4772,7 @@
       </c>
       <c r="F56" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
@@ -4759,13 +4781,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K56" s="4" t="e">
-        <f>VLOOKUP(C56,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L56" s="5" t="e">
+      <c r="K56" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C56,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L56" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M56" s="4">
         <f t="shared" si="13"/>
@@ -4803,7 +4825,7 @@
       </c>
       <c r="F57" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
@@ -4812,13 +4834,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K57" s="4" t="e">
-        <f>VLOOKUP(C57,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L57" s="5" t="e">
+      <c r="K57" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C57,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L57" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M57" s="4">
         <f t="shared" si="13"/>
@@ -4856,7 +4878,7 @@
       </c>
       <c r="F58" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
@@ -4865,13 +4887,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K58" s="4" t="e">
-        <f>VLOOKUP(C58,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L58" s="5" t="e">
+      <c r="K58" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C58,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L58" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M58" s="4">
         <f t="shared" si="13"/>
@@ -4909,7 +4931,7 @@
       </c>
       <c r="F59" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
@@ -4918,13 +4940,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K59" s="4" t="e">
-        <f>VLOOKUP(C59,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L59" s="5" t="e">
+      <c r="K59" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C59,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L59" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M59" s="4">
         <f t="shared" si="13"/>
@@ -4962,7 +4984,7 @@
       </c>
       <c r="F60" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
@@ -4971,13 +4993,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K60" s="4" t="e">
-        <f>VLOOKUP(C60,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L60" s="5" t="e">
+      <c r="K60" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C60,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L60" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M60" s="4">
         <f t="shared" si="13"/>
@@ -5015,7 +5037,7 @@
       </c>
       <c r="F61" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
@@ -5024,13 +5046,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K61" s="4" t="e">
-        <f>VLOOKUP(C61,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L61" s="5" t="e">
+      <c r="K61" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C61,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L61" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M61" s="4">
         <f t="shared" si="13"/>
@@ -5068,7 +5090,7 @@
       </c>
       <c r="F62" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
@@ -5077,13 +5099,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K62" s="4" t="e">
-        <f>VLOOKUP(C62,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L62" s="5" t="e">
+      <c r="K62" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C62,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L62" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M62" s="4">
         <f t="shared" si="13"/>
@@ -5121,7 +5143,7 @@
       </c>
       <c r="F63" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
@@ -5130,13 +5152,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K63" s="4" t="e">
-        <f>VLOOKUP(C63,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L63" s="5" t="e">
+      <c r="K63" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C63,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L63" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M63" s="4">
         <f t="shared" si="13"/>
@@ -5174,7 +5196,7 @@
       </c>
       <c r="F64" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
@@ -5183,13 +5205,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K64" s="4" t="e">
-        <f>VLOOKUP(C64,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L64" s="5" t="e">
+      <c r="K64" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C64,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L64" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M64" s="4">
         <f t="shared" si="13"/>
@@ -5227,7 +5249,7 @@
       </c>
       <c r="F65" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
@@ -5236,13 +5258,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K65" s="4" t="e">
-        <f>VLOOKUP(C65,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L65" s="5" t="e">
+      <c r="K65" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C65,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L65" s="5" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M65" s="4">
         <f t="shared" si="13"/>
@@ -5280,7 +5302,7 @@
       </c>
       <c r="F66" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
@@ -5289,13 +5311,13 @@
         <f t="shared" ca="1" si="7"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K66" s="4" t="e">
-        <f>VLOOKUP(C66,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L66" s="5" t="e">
+      <c r="K66" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C66,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L66" s="5" t="str">
         <f t="shared" ref="L66:L69" si="14">IF(EXACT(K66,E66),"ü","x")</f>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M66" s="4">
         <f t="shared" si="13"/>
@@ -5333,7 +5355,7 @@
       </c>
       <c r="F67" s="3">
         <f t="shared" ref="F67:F69" ca="1" si="15">TODAY()</f>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
@@ -5342,13 +5364,13 @@
         <f t="shared" ref="J67:J69" ca="1" si="16">CONCATENATE(TEXT(A67,"0")," - ","CCMA - ",YEAR(F67)&amp;TEXT(MONTH(F67),"00")," - ",SUBSTITUTE(D67,"-","")," - ",B67)</f>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K67" s="4" t="e">
-        <f>VLOOKUP(C67,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L67" s="5" t="e">
+      <c r="K67" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C67,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L67" s="5" t="str">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M67" s="4">
         <f t="shared" si="13"/>
@@ -5386,7 +5408,7 @@
       </c>
       <c r="F68" s="3">
         <f t="shared" ca="1" si="15"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
@@ -5395,13 +5417,13 @@
         <f t="shared" ca="1" si="16"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K68" s="4" t="e">
-        <f>VLOOKUP(C68,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L68" s="5" t="e">
+      <c r="K68" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C68,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L68" s="5" t="str">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M68" s="4">
         <f t="shared" si="13"/>
@@ -5439,7 +5461,7 @@
       </c>
       <c r="F69" s="3">
         <f t="shared" ca="1" si="15"/>
-        <v>45109</v>
+        <v>45111</v>
       </c>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
@@ -5448,13 +5470,13 @@
         <f t="shared" ca="1" si="16"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
-      <c r="K69" s="4" t="e">
-        <f>VLOOKUP(C69,[1]Hoja1!$J:$L,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L69" s="5" t="e">
+      <c r="K69" s="4" t="str">
+        <f>_xlfn.IFNA(VLOOKUP(C69,[1]Hoja1!$J:$L,3,0),"")</f>
+        <v/>
+      </c>
+      <c r="L69" s="5" t="str">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
+        <v>x</v>
       </c>
       <c r="M69" s="4">
         <f t="shared" si="13"/>

</xml_diff>

<commit_message>
Update: Add Taxprayer selector
</commit_message>
<xml_diff>
--- a/CCMA.xlsx
+++ b/CCMA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\Descarga_CCMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA596932-A2A4-4539-B60D-F00643045589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D3E97D-B9C6-4EB9-861D-063CC5B1AD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="17">
   <si>
     <t>Nro</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>Con anterior y posterior</t>
-  </si>
-  <si>
-    <t>30-00000000-0</t>
   </si>
   <si>
     <t>Clave</t>
@@ -1822,7 +1819,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1856,19 +1853,19 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -1901,15 +1898,15 @@
         <v>20000000000</v>
       </c>
       <c r="D2" t="str">
-        <f>TEXT(C2,"00-00000000-0")</f>
-        <v>20-00000000-0</v>
+        <f>TEXT(C2,"00000000000")</f>
+        <v>20000000000</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" s="3">
         <f ca="1">TODAY()</f>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -1955,15 +1952,15 @@
         <v>20000000000</v>
       </c>
       <c r="D3" t="str">
-        <f>TEXT(C3,"00-00000000-0")</f>
-        <v>20-00000000-0</v>
+        <f>TEXT(C3,"00000000000")</f>
+        <v>20000000000</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F66" ca="1" si="6">TODAY()</f>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -2008,15 +2005,15 @@
       <c r="C4">
         <v>20000000000</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
+      <c r="D4">
+        <v>30000000000</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -2061,15 +2058,15 @@
       <c r="C5">
         <v>20000000000</v>
       </c>
-      <c r="D5" t="s">
-        <v>12</v>
+      <c r="D5">
+        <v>30000000000</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -2114,15 +2111,15 @@
       <c r="C6">
         <v>20000000000</v>
       </c>
-      <c r="D6" t="s">
-        <v>12</v>
+      <c r="D6">
+        <v>30000000000</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -2167,15 +2164,15 @@
       <c r="C7">
         <v>20000000000</v>
       </c>
-      <c r="D7" t="s">
-        <v>12</v>
+      <c r="D7">
+        <v>30000000000</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -2220,15 +2217,15 @@
       <c r="C8">
         <v>20000000000</v>
       </c>
-      <c r="D8" t="s">
-        <v>12</v>
+      <c r="D8">
+        <v>30000000000</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -2273,15 +2270,15 @@
       <c r="C9">
         <v>20000000000</v>
       </c>
-      <c r="D9" t="s">
-        <v>12</v>
+      <c r="D9">
+        <v>30000000000</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -2326,15 +2323,15 @@
       <c r="C10">
         <v>20000000000</v>
       </c>
-      <c r="D10" t="s">
-        <v>12</v>
+      <c r="D10">
+        <v>30000000000</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -2379,15 +2376,15 @@
       <c r="C11">
         <v>20000000000</v>
       </c>
-      <c r="D11" t="s">
-        <v>12</v>
+      <c r="D11">
+        <v>30000000000</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -2432,15 +2429,15 @@
       <c r="C12">
         <v>20000000000</v>
       </c>
-      <c r="D12" t="s">
-        <v>12</v>
+      <c r="D12">
+        <v>30000000000</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -2485,15 +2482,15 @@
       <c r="C13">
         <v>20000000000</v>
       </c>
-      <c r="D13" t="s">
-        <v>12</v>
+      <c r="D13">
+        <v>30000000000</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -2538,15 +2535,15 @@
       <c r="C14">
         <v>20000000000</v>
       </c>
-      <c r="D14" t="s">
-        <v>12</v>
+      <c r="D14">
+        <v>30000000000</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -2591,15 +2588,15 @@
       <c r="C15">
         <v>20000000000</v>
       </c>
-      <c r="D15" t="s">
-        <v>12</v>
+      <c r="D15">
+        <v>30000000000</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -2644,15 +2641,15 @@
       <c r="C16">
         <v>20000000000</v>
       </c>
-      <c r="D16" t="s">
-        <v>12</v>
+      <c r="D16">
+        <v>30000000000</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -2697,15 +2694,15 @@
       <c r="C17">
         <v>20000000000</v>
       </c>
-      <c r="D17" t="s">
-        <v>12</v>
+      <c r="D17">
+        <v>30000000000</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -2750,15 +2747,15 @@
       <c r="C18">
         <v>20000000000</v>
       </c>
-      <c r="D18" t="s">
-        <v>12</v>
+      <c r="D18">
+        <v>30000000000</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -2803,15 +2800,15 @@
       <c r="C19">
         <v>20000000000</v>
       </c>
-      <c r="D19" t="s">
-        <v>12</v>
+      <c r="D19">
+        <v>30000000000</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -2856,15 +2853,15 @@
       <c r="C20">
         <v>20000000000</v>
       </c>
-      <c r="D20" t="s">
-        <v>12</v>
+      <c r="D20">
+        <v>30000000000</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -2909,15 +2906,15 @@
       <c r="C21">
         <v>20000000000</v>
       </c>
-      <c r="D21" t="s">
-        <v>12</v>
+      <c r="D21">
+        <v>30000000000</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -2962,15 +2959,15 @@
       <c r="C22">
         <v>20000000000</v>
       </c>
-      <c r="D22" t="s">
-        <v>12</v>
+      <c r="D22">
+        <v>30000000000</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -3015,15 +3012,15 @@
       <c r="C23">
         <v>20000000000</v>
       </c>
-      <c r="D23" t="s">
-        <v>12</v>
+      <c r="D23">
+        <v>30000000000</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -3068,15 +3065,15 @@
       <c r="C24">
         <v>20000000000</v>
       </c>
-      <c r="D24" t="s">
-        <v>12</v>
+      <c r="D24">
+        <v>30000000000</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -3121,15 +3118,15 @@
       <c r="C25">
         <v>20000000000</v>
       </c>
-      <c r="D25" t="s">
-        <v>12</v>
+      <c r="D25">
+        <v>30000000000</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -3174,15 +3171,15 @@
       <c r="C26">
         <v>20000000000</v>
       </c>
-      <c r="D26" t="s">
-        <v>12</v>
+      <c r="D26">
+        <v>30000000000</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -3227,15 +3224,15 @@
       <c r="C27">
         <v>20000000000</v>
       </c>
-      <c r="D27" t="s">
-        <v>12</v>
+      <c r="D27">
+        <v>30000000000</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -3280,15 +3277,15 @@
       <c r="C28">
         <v>20000000000</v>
       </c>
-      <c r="D28" t="s">
-        <v>12</v>
+      <c r="D28">
+        <v>30000000000</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -3333,15 +3330,15 @@
       <c r="C29">
         <v>20000000000</v>
       </c>
-      <c r="D29" t="s">
-        <v>12</v>
+      <c r="D29">
+        <v>30000000000</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -3386,15 +3383,15 @@
       <c r="C30">
         <v>20000000000</v>
       </c>
-      <c r="D30" t="s">
-        <v>12</v>
+      <c r="D30">
+        <v>30000000000</v>
       </c>
       <c r="E30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -3439,15 +3436,15 @@
       <c r="C31">
         <v>20000000000</v>
       </c>
-      <c r="D31" t="s">
-        <v>12</v>
+      <c r="D31">
+        <v>30000000000</v>
       </c>
       <c r="E31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F31" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -3492,15 +3489,15 @@
       <c r="C32">
         <v>20000000000</v>
       </c>
-      <c r="D32" t="s">
-        <v>12</v>
+      <c r="D32">
+        <v>30000000000</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F32" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -3545,15 +3542,15 @@
       <c r="C33">
         <v>20000000000</v>
       </c>
-      <c r="D33" t="s">
-        <v>12</v>
+      <c r="D33">
+        <v>30000000000</v>
       </c>
       <c r="E33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F33" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -3598,15 +3595,15 @@
       <c r="C34">
         <v>20000000000</v>
       </c>
-      <c r="D34" t="s">
-        <v>12</v>
+      <c r="D34">
+        <v>30000000000</v>
       </c>
       <c r="E34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F34" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -3651,15 +3648,15 @@
       <c r="C35">
         <v>20000000000</v>
       </c>
-      <c r="D35" t="s">
-        <v>12</v>
+      <c r="D35">
+        <v>30000000000</v>
       </c>
       <c r="E35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F35" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -3704,15 +3701,15 @@
       <c r="C36">
         <v>20000000000</v>
       </c>
-      <c r="D36" t="s">
-        <v>12</v>
+      <c r="D36">
+        <v>30000000000</v>
       </c>
       <c r="E36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F36" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -3757,15 +3754,15 @@
       <c r="C37">
         <v>20000000000</v>
       </c>
-      <c r="D37" t="s">
-        <v>12</v>
+      <c r="D37">
+        <v>30000000000</v>
       </c>
       <c r="E37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F37" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -3810,15 +3807,15 @@
       <c r="C38">
         <v>20000000000</v>
       </c>
-      <c r="D38" t="s">
-        <v>12</v>
+      <c r="D38">
+        <v>30000000000</v>
       </c>
       <c r="E38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F38" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -3863,15 +3860,15 @@
       <c r="C39">
         <v>20000000000</v>
       </c>
-      <c r="D39" t="s">
-        <v>12</v>
+      <c r="D39">
+        <v>30000000000</v>
       </c>
       <c r="E39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F39" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -3916,15 +3913,15 @@
       <c r="C40">
         <v>20000000000</v>
       </c>
-      <c r="D40" t="s">
-        <v>12</v>
+      <c r="D40">
+        <v>30000000000</v>
       </c>
       <c r="E40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F40" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
@@ -3969,15 +3966,15 @@
       <c r="C41">
         <v>20000000000</v>
       </c>
-      <c r="D41" t="s">
-        <v>12</v>
+      <c r="D41">
+        <v>30000000000</v>
       </c>
       <c r="E41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F41" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -4022,15 +4019,15 @@
       <c r="C42">
         <v>20000000000</v>
       </c>
-      <c r="D42" t="s">
-        <v>12</v>
+      <c r="D42">
+        <v>30000000000</v>
       </c>
       <c r="E42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F42" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -4075,15 +4072,15 @@
       <c r="C43">
         <v>20000000000</v>
       </c>
-      <c r="D43" t="s">
-        <v>12</v>
+      <c r="D43">
+        <v>30000000000</v>
       </c>
       <c r="E43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F43" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -4128,15 +4125,15 @@
       <c r="C44">
         <v>20000000000</v>
       </c>
-      <c r="D44" t="s">
-        <v>12</v>
+      <c r="D44">
+        <v>30000000000</v>
       </c>
       <c r="E44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F44" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -4181,15 +4178,15 @@
       <c r="C45">
         <v>20000000000</v>
       </c>
-      <c r="D45" t="s">
-        <v>12</v>
+      <c r="D45">
+        <v>30000000000</v>
       </c>
       <c r="E45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F45" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -4234,15 +4231,15 @@
       <c r="C46">
         <v>20000000000</v>
       </c>
-      <c r="D46" t="s">
-        <v>12</v>
+      <c r="D46">
+        <v>30000000000</v>
       </c>
       <c r="E46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F46" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -4287,15 +4284,15 @@
       <c r="C47">
         <v>20000000000</v>
       </c>
-      <c r="D47" t="s">
-        <v>12</v>
+      <c r="D47">
+        <v>30000000000</v>
       </c>
       <c r="E47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F47" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -4340,15 +4337,15 @@
       <c r="C48">
         <v>20000000000</v>
       </c>
-      <c r="D48" t="s">
-        <v>12</v>
+      <c r="D48">
+        <v>30000000000</v>
       </c>
       <c r="E48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F48" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
@@ -4393,15 +4390,15 @@
       <c r="C49">
         <v>20000000000</v>
       </c>
-      <c r="D49" t="s">
-        <v>12</v>
+      <c r="D49">
+        <v>30000000000</v>
       </c>
       <c r="E49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F49" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
@@ -4446,15 +4443,15 @@
       <c r="C50">
         <v>20000000000</v>
       </c>
-      <c r="D50" t="s">
-        <v>12</v>
+      <c r="D50">
+        <v>30000000000</v>
       </c>
       <c r="E50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F50" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -4499,15 +4496,15 @@
       <c r="C51">
         <v>20000000000</v>
       </c>
-      <c r="D51" t="s">
-        <v>12</v>
+      <c r="D51">
+        <v>30000000000</v>
       </c>
       <c r="E51" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F51" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -4552,15 +4549,15 @@
       <c r="C52">
         <v>20000000000</v>
       </c>
-      <c r="D52" t="s">
-        <v>12</v>
+      <c r="D52">
+        <v>30000000000</v>
       </c>
       <c r="E52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F52" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -4605,15 +4602,15 @@
       <c r="C53">
         <v>20000000000</v>
       </c>
-      <c r="D53" t="s">
-        <v>12</v>
+      <c r="D53">
+        <v>30000000000</v>
       </c>
       <c r="E53" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F53" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
@@ -4658,15 +4655,15 @@
       <c r="C54">
         <v>20000000000</v>
       </c>
-      <c r="D54" t="s">
-        <v>12</v>
+      <c r="D54">
+        <v>30000000000</v>
       </c>
       <c r="E54" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F54" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
@@ -4711,15 +4708,15 @@
       <c r="C55">
         <v>20000000000</v>
       </c>
-      <c r="D55" t="s">
-        <v>12</v>
+      <c r="D55">
+        <v>30000000000</v>
       </c>
       <c r="E55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F55" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
@@ -4764,15 +4761,15 @@
       <c r="C56">
         <v>20000000000</v>
       </c>
-      <c r="D56" t="s">
-        <v>12</v>
+      <c r="D56">
+        <v>30000000000</v>
       </c>
       <c r="E56" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F56" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
@@ -4817,15 +4814,15 @@
       <c r="C57">
         <v>20000000000</v>
       </c>
-      <c r="D57" t="s">
-        <v>12</v>
+      <c r="D57">
+        <v>30000000000</v>
       </c>
       <c r="E57" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F57" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
@@ -4870,15 +4867,15 @@
       <c r="C58">
         <v>20000000000</v>
       </c>
-      <c r="D58" t="s">
-        <v>12</v>
+      <c r="D58">
+        <v>30000000000</v>
       </c>
       <c r="E58" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F58" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
@@ -4923,15 +4920,15 @@
       <c r="C59">
         <v>20000000000</v>
       </c>
-      <c r="D59" t="s">
-        <v>12</v>
+      <c r="D59">
+        <v>30000000000</v>
       </c>
       <c r="E59" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F59" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
@@ -4976,15 +4973,15 @@
       <c r="C60">
         <v>20000000000</v>
       </c>
-      <c r="D60" t="s">
-        <v>12</v>
+      <c r="D60">
+        <v>30000000000</v>
       </c>
       <c r="E60" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F60" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
@@ -5029,15 +5026,15 @@
       <c r="C61">
         <v>20000000000</v>
       </c>
-      <c r="D61" t="s">
-        <v>12</v>
+      <c r="D61">
+        <v>30000000000</v>
       </c>
       <c r="E61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F61" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
@@ -5082,15 +5079,15 @@
       <c r="C62">
         <v>20000000000</v>
       </c>
-      <c r="D62" t="s">
-        <v>12</v>
+      <c r="D62">
+        <v>30000000000</v>
       </c>
       <c r="E62" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F62" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
@@ -5135,15 +5132,15 @@
       <c r="C63">
         <v>20000000000</v>
       </c>
-      <c r="D63" t="s">
-        <v>12</v>
+      <c r="D63">
+        <v>30000000000</v>
       </c>
       <c r="E63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F63" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
@@ -5188,15 +5185,15 @@
       <c r="C64">
         <v>20000000000</v>
       </c>
-      <c r="D64" t="s">
-        <v>12</v>
+      <c r="D64">
+        <v>30000000000</v>
       </c>
       <c r="E64" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F64" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
@@ -5241,15 +5238,15 @@
       <c r="C65">
         <v>20000000000</v>
       </c>
-      <c r="D65" t="s">
-        <v>12</v>
+      <c r="D65">
+        <v>30000000000</v>
       </c>
       <c r="E65" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F65" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
@@ -5294,15 +5291,15 @@
       <c r="C66">
         <v>20000000000</v>
       </c>
-      <c r="D66" t="s">
-        <v>12</v>
+      <c r="D66">
+        <v>30000000000</v>
       </c>
       <c r="E66" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F66" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
@@ -5347,15 +5344,15 @@
       <c r="C67">
         <v>20000000000</v>
       </c>
-      <c r="D67" t="s">
-        <v>12</v>
+      <c r="D67">
+        <v>30000000000</v>
       </c>
       <c r="E67" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F67" s="3">
         <f t="shared" ref="F67:F69" ca="1" si="15">TODAY()</f>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
@@ -5400,15 +5397,15 @@
       <c r="C68">
         <v>20000000000</v>
       </c>
-      <c r="D68" t="s">
-        <v>12</v>
+      <c r="D68">
+        <v>30000000000</v>
       </c>
       <c r="E68" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F68" s="3">
         <f t="shared" ca="1" si="15"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
@@ -5453,15 +5450,15 @@
       <c r="C69">
         <v>20000000000</v>
       </c>
-      <c r="D69" t="s">
-        <v>12</v>
+      <c r="D69">
+        <v>30000000000</v>
       </c>
       <c r="E69" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F69" s="3">
         <f t="shared" ca="1" si="15"/>
-        <v>45111</v>
+        <v>45125</v>
       </c>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>

</xml_diff>

<commit_message>
Adapt for future feature of new control
</commit_message>
<xml_diff>
--- a/CCMA.xlsx
+++ b/CCMA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\Descarga_CCMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D3E97D-B9C6-4EB9-861D-063CC5B1AD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80321D5C-3A25-470D-9167-493B2D089605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Listado!$A$1:$P$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Listado!$A$1:$N$69</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="15">
   <si>
     <t>Nro</t>
   </si>
@@ -79,12 +79,6 @@
   </si>
   <si>
     <t>Clave</t>
-  </si>
-  <si>
-    <t>Raiz</t>
-  </si>
-  <si>
-    <t>Ubicación Descarga</t>
   </si>
   <si>
     <t>CCMA</t>
@@ -1815,11 +1809,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P69"/>
+  <dimension ref="A1:N69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1829,14 +1823,14 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="14.5703125" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1853,7 +1847,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -1862,31 +1856,25 @@
         <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f t="shared" ref="A2:A33" si="0">RIGHT(D2,1)</f>
         <v>0</v>
@@ -1906,41 +1894,39 @@
       </c>
       <c r="F2" s="3">
         <f ca="1">TODAY()</f>
-        <v>45125</v>
+        <v>45131</v>
       </c>
       <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="2" t="str">
+      <c r="H2" s="2" t="str">
         <f ca="1">CONCATENATE(TEXT(A2,"0")," - ","CCMA - ",YEAR(F2)&amp;TEXT(MONTH(F2),"00")," - ",SUBSTITUTE(D2,"-","")," - ",B2)</f>
         <v>0 - CCMA - 202307 - 20000000000 - Cliente</v>
       </c>
-      <c r="K2" s="4" t="str">
+      <c r="I2" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C2,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L2" s="5" t="str">
-        <f t="shared" ref="L2:L33" si="1">IF(EXACT(K2,E2),"ü","x")</f>
-        <v>x</v>
+      <c r="J2" s="5" t="str">
+        <f>IF(EXACT(I2,E2),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K2" s="4">
+        <f>ROW(A2)</f>
+        <v>2</v>
+      </c>
+      <c r="L2" s="4">
+        <f>IF(C2=C1,1,0)</f>
+        <v>0</v>
       </c>
       <c r="M2" s="4">
-        <f t="shared" ref="M2:M33" si="2">ROW(A2)</f>
-        <v>2</v>
+        <f>IF(C2=C3,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N2" s="4">
-        <f t="shared" ref="N2" si="3">IF(C2=C1,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O2" s="4">
-        <f t="shared" ref="O2" si="4">IF(C2=C3,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="P2" s="4">
-        <f t="shared" ref="P2" si="5">SUM(N2:O2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" ref="N2" si="1">SUM(L2:M2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1959,42 +1945,40 @@
         <v>12</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F66" ca="1" si="6">TODAY()</f>
-        <v>45125</v>
+        <f t="shared" ref="F3:F66" ca="1" si="2">TODAY()</f>
+        <v>45131</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="2" t="str">
-        <f t="shared" ref="J3:J66" ca="1" si="7">CONCATENATE(TEXT(A3,"0")," - ","CCMA - ",YEAR(F3)&amp;TEXT(MONTH(F3),"00")," - ",SUBSTITUTE(D3,"-","")," - ",B3)</f>
+      <c r="H3" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A3,"0")," - ","CCMA - ",YEAR(F3)&amp;TEXT(MONTH(F3),"00")," - ",SUBSTITUTE(D3,"-","")," - ",B3)</f>
         <v>0 - CCMA - 202307 - 20000000000 - Cliente</v>
       </c>
-      <c r="K3" s="4" t="str">
+      <c r="I3" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C3,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L3" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J3" s="5" t="str">
+        <f>IF(EXACT(I3,E3),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K3" s="4">
+        <f>ROW(A3)</f>
+        <v>3</v>
+      </c>
+      <c r="L3" s="4">
+        <f>IF(C3=C2,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M3" s="4">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f>IF(C3=C4,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N3" s="4">
-        <f t="shared" ref="N3:N66" si="8">IF(C3=C2,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="O3" s="4">
-        <f t="shared" ref="O3:O66" si="9">IF(C3=C4,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="P3" s="4">
-        <f t="shared" ref="P3:P66" si="10">SUM(N3:O3)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" ref="N3:N66" si="3">SUM(L3:M3)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2012,42 +1996,40 @@
         <v>12</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K4" s="4" t="str">
+      <c r="H4" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A4,"0")," - ","CCMA - ",YEAR(F4)&amp;TEXT(MONTH(F4),"00")," - ",SUBSTITUTE(D4,"-","")," - ",B4)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I4" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C4,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L4" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J4" s="5" t="str">
+        <f>IF(EXACT(I4,E4),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K4" s="4">
+        <f>ROW(A4)</f>
+        <v>4</v>
+      </c>
+      <c r="L4" s="4">
+        <f>IF(C4=C3,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M4" s="4">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f>IF(C4=C5,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N4" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O4" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P4" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2065,42 +2047,40 @@
         <v>12</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K5" s="4" t="str">
+      <c r="H5" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A5,"0")," - ","CCMA - ",YEAR(F5)&amp;TEXT(MONTH(F5),"00")," - ",SUBSTITUTE(D5,"-","")," - ",B5)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I5" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C5,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L5" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J5" s="5" t="str">
+        <f>IF(EXACT(I5,E5),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K5" s="4">
+        <f>ROW(A5)</f>
+        <v>5</v>
+      </c>
+      <c r="L5" s="4">
+        <f>IF(C5=C4,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M5" s="4">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f>IF(C5=C6,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O5" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P5" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2118,42 +2098,40 @@
         <v>12</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K6" s="4" t="str">
+      <c r="H6" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A6,"0")," - ","CCMA - ",YEAR(F6)&amp;TEXT(MONTH(F6),"00")," - ",SUBSTITUTE(D6,"-","")," - ",B6)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I6" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C6,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L6" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J6" s="5" t="str">
+        <f>IF(EXACT(I6,E6),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K6" s="4">
+        <f>ROW(A6)</f>
+        <v>6</v>
+      </c>
+      <c r="L6" s="4">
+        <f>IF(C6=C5,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M6" s="4">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f>IF(C6=C7,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O6" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P6" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2171,42 +2149,40 @@
         <v>12</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K7" s="4" t="str">
+      <c r="H7" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A7,"0")," - ","CCMA - ",YEAR(F7)&amp;TEXT(MONTH(F7),"00")," - ",SUBSTITUTE(D7,"-","")," - ",B7)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I7" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C7,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L7" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J7" s="5" t="str">
+        <f>IF(EXACT(I7,E7),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K7" s="4">
+        <f>ROW(A7)</f>
+        <v>7</v>
+      </c>
+      <c r="L7" s="4">
+        <f>IF(C7=C6,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M7" s="4">
-        <f t="shared" si="2"/>
-        <v>7</v>
+        <f>IF(C7=C8,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O7" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P7" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2224,42 +2200,40 @@
         <v>12</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K8" s="4" t="str">
+      <c r="H8" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A8,"0")," - ","CCMA - ",YEAR(F8)&amp;TEXT(MONTH(F8),"00")," - ",SUBSTITUTE(D8,"-","")," - ",B8)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I8" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C8,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L8" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J8" s="5" t="str">
+        <f>IF(EXACT(I8,E8),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K8" s="4">
+        <f>ROW(A8)</f>
+        <v>8</v>
+      </c>
+      <c r="L8" s="4">
+        <f>IF(C8=C7,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M8" s="4">
-        <f t="shared" si="2"/>
-        <v>8</v>
+        <f>IF(C8=C9,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N8" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O8" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P8" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2277,42 +2251,40 @@
         <v>12</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K9" s="4" t="str">
+      <c r="H9" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A9,"0")," - ","CCMA - ",YEAR(F9)&amp;TEXT(MONTH(F9),"00")," - ",SUBSTITUTE(D9,"-","")," - ",B9)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I9" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C9,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L9" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J9" s="5" t="str">
+        <f>IF(EXACT(I9,E9),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K9" s="4">
+        <f>ROW(A9)</f>
+        <v>9</v>
+      </c>
+      <c r="L9" s="4">
+        <f>IF(C9=C8,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M9" s="4">
-        <f t="shared" si="2"/>
-        <v>9</v>
+        <f>IF(C9=C10,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N9" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O9" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P9" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2330,42 +2302,40 @@
         <v>12</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K10" s="4" t="str">
+      <c r="H10" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A10,"0")," - ","CCMA - ",YEAR(F10)&amp;TEXT(MONTH(F10),"00")," - ",SUBSTITUTE(D10,"-","")," - ",B10)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I10" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C10,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L10" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J10" s="5" t="str">
+        <f>IF(EXACT(I10,E10),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K10" s="4">
+        <f>ROW(A10)</f>
+        <v>10</v>
+      </c>
+      <c r="L10" s="4">
+        <f>IF(C10=C9,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M10" s="4">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <f>IF(C10=C11,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N10" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O10" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P10" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2383,42 +2353,40 @@
         <v>12</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K11" s="4" t="str">
+      <c r="H11" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A11,"0")," - ","CCMA - ",YEAR(F11)&amp;TEXT(MONTH(F11),"00")," - ",SUBSTITUTE(D11,"-","")," - ",B11)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I11" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C11,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L11" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J11" s="5" t="str">
+        <f>IF(EXACT(I11,E11),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K11" s="4">
+        <f>ROW(A11)</f>
+        <v>11</v>
+      </c>
+      <c r="L11" s="4">
+        <f>IF(C11=C10,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M11" s="4">
-        <f t="shared" si="2"/>
-        <v>11</v>
+        <f>IF(C11=C12,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O11" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P11" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2436,42 +2404,40 @@
         <v>12</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K12" s="4" t="str">
+      <c r="H12" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A12,"0")," - ","CCMA - ",YEAR(F12)&amp;TEXT(MONTH(F12),"00")," - ",SUBSTITUTE(D12,"-","")," - ",B12)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I12" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C12,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L12" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J12" s="5" t="str">
+        <f>IF(EXACT(I12,E12),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K12" s="4">
+        <f>ROW(A12)</f>
+        <v>12</v>
+      </c>
+      <c r="L12" s="4">
+        <f>IF(C12=C11,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M12" s="4">
-        <f t="shared" si="2"/>
-        <v>12</v>
+        <f>IF(C12=C13,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N12" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O12" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P12" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2489,42 +2455,40 @@
         <v>12</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K13" s="4" t="str">
+      <c r="H13" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A13,"0")," - ","CCMA - ",YEAR(F13)&amp;TEXT(MONTH(F13),"00")," - ",SUBSTITUTE(D13,"-","")," - ",B13)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I13" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C13,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L13" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J13" s="5" t="str">
+        <f>IF(EXACT(I13,E13),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K13" s="4">
+        <f>ROW(A13)</f>
+        <v>13</v>
+      </c>
+      <c r="L13" s="4">
+        <f>IF(C13=C12,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M13" s="4">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <f>IF(C13=C14,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N13" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O13" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P13" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2542,42 +2506,40 @@
         <v>12</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K14" s="4" t="str">
+      <c r="H14" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A14,"0")," - ","CCMA - ",YEAR(F14)&amp;TEXT(MONTH(F14),"00")," - ",SUBSTITUTE(D14,"-","")," - ",B14)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I14" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C14,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L14" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J14" s="5" t="str">
+        <f>IF(EXACT(I14,E14),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K14" s="4">
+        <f>ROW(A14)</f>
+        <v>14</v>
+      </c>
+      <c r="L14" s="4">
+        <f>IF(C14=C13,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M14" s="4">
-        <f t="shared" si="2"/>
-        <v>14</v>
+        <f>IF(C14=C15,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N14" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O14" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P14" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2595,42 +2557,40 @@
         <v>12</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K15" s="4" t="str">
+      <c r="H15" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A15,"0")," - ","CCMA - ",YEAR(F15)&amp;TEXT(MONTH(F15),"00")," - ",SUBSTITUTE(D15,"-","")," - ",B15)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I15" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C15,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L15" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J15" s="5" t="str">
+        <f>IF(EXACT(I15,E15),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K15" s="4">
+        <f>ROW(A15)</f>
+        <v>15</v>
+      </c>
+      <c r="L15" s="4">
+        <f>IF(C15=C14,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M15" s="4">
-        <f t="shared" si="2"/>
-        <v>15</v>
+        <f>IF(C15=C16,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N15" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O15" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P15" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2648,42 +2608,40 @@
         <v>12</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K16" s="4" t="str">
+      <c r="H16" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A16,"0")," - ","CCMA - ",YEAR(F16)&amp;TEXT(MONTH(F16),"00")," - ",SUBSTITUTE(D16,"-","")," - ",B16)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I16" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C16,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L16" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J16" s="5" t="str">
+        <f>IF(EXACT(I16,E16),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K16" s="4">
+        <f>ROW(A16)</f>
+        <v>16</v>
+      </c>
+      <c r="L16" s="4">
+        <f>IF(C16=C15,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M16" s="4">
-        <f t="shared" si="2"/>
-        <v>16</v>
+        <f>IF(C16=C17,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N16" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O16" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P16" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2701,42 +2659,40 @@
         <v>12</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K17" s="4" t="str">
+      <c r="H17" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A17,"0")," - ","CCMA - ",YEAR(F17)&amp;TEXT(MONTH(F17),"00")," - ",SUBSTITUTE(D17,"-","")," - ",B17)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I17" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C17,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L17" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J17" s="5" t="str">
+        <f>IF(EXACT(I17,E17),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K17" s="4">
+        <f>ROW(A17)</f>
+        <v>17</v>
+      </c>
+      <c r="L17" s="4">
+        <f>IF(C17=C16,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M17" s="4">
-        <f t="shared" si="2"/>
-        <v>17</v>
+        <f>IF(C17=C18,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N17" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O17" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P17" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2754,42 +2710,40 @@
         <v>12</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K18" s="4" t="str">
+      <c r="H18" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A18,"0")," - ","CCMA - ",YEAR(F18)&amp;TEXT(MONTH(F18),"00")," - ",SUBSTITUTE(D18,"-","")," - ",B18)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I18" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C18,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L18" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J18" s="5" t="str">
+        <f>IF(EXACT(I18,E18),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K18" s="4">
+        <f>ROW(A18)</f>
+        <v>18</v>
+      </c>
+      <c r="L18" s="4">
+        <f>IF(C18=C17,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M18" s="4">
-        <f t="shared" si="2"/>
-        <v>18</v>
+        <f>IF(C18=C19,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N18" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O18" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P18" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2807,42 +2761,40 @@
         <v>12</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K19" s="4" t="str">
+      <c r="H19" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A19,"0")," - ","CCMA - ",YEAR(F19)&amp;TEXT(MONTH(F19),"00")," - ",SUBSTITUTE(D19,"-","")," - ",B19)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I19" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C19,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L19" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J19" s="5" t="str">
+        <f>IF(EXACT(I19,E19),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K19" s="4">
+        <f>ROW(A19)</f>
+        <v>19</v>
+      </c>
+      <c r="L19" s="4">
+        <f>IF(C19=C18,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M19" s="4">
-        <f t="shared" si="2"/>
-        <v>19</v>
+        <f>IF(C19=C20,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N19" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O19" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P19" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2860,42 +2812,40 @@
         <v>12</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K20" s="4" t="str">
+      <c r="H20" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A20,"0")," - ","CCMA - ",YEAR(F20)&amp;TEXT(MONTH(F20),"00")," - ",SUBSTITUTE(D20,"-","")," - ",B20)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I20" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C20,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L20" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J20" s="5" t="str">
+        <f>IF(EXACT(I20,E20),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K20" s="4">
+        <f>ROW(A20)</f>
+        <v>20</v>
+      </c>
+      <c r="L20" s="4">
+        <f>IF(C20=C19,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M20" s="4">
-        <f t="shared" si="2"/>
-        <v>20</v>
+        <f>IF(C20=C21,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N20" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O20" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P20" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2913,42 +2863,40 @@
         <v>12</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K21" s="4" t="str">
+      <c r="H21" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A21,"0")," - ","CCMA - ",YEAR(F21)&amp;TEXT(MONTH(F21),"00")," - ",SUBSTITUTE(D21,"-","")," - ",B21)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I21" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C21,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L21" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J21" s="5" t="str">
+        <f>IF(EXACT(I21,E21),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K21" s="4">
+        <f>ROW(A21)</f>
+        <v>21</v>
+      </c>
+      <c r="L21" s="4">
+        <f>IF(C21=C20,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M21" s="4">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f>IF(C21=C22,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N21" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O21" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P21" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2966,42 +2914,40 @@
         <v>12</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K22" s="4" t="str">
+      <c r="H22" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A22,"0")," - ","CCMA - ",YEAR(F22)&amp;TEXT(MONTH(F22),"00")," - ",SUBSTITUTE(D22,"-","")," - ",B22)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I22" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C22,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L22" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J22" s="5" t="str">
+        <f>IF(EXACT(I22,E22),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K22" s="4">
+        <f>ROW(A22)</f>
+        <v>22</v>
+      </c>
+      <c r="L22" s="4">
+        <f>IF(C22=C21,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M22" s="4">
-        <f t="shared" si="2"/>
-        <v>22</v>
+        <f>IF(C22=C23,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N22" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O22" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P22" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3019,42 +2965,40 @@
         <v>12</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K23" s="4" t="str">
+      <c r="H23" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A23,"0")," - ","CCMA - ",YEAR(F23)&amp;TEXT(MONTH(F23),"00")," - ",SUBSTITUTE(D23,"-","")," - ",B23)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I23" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C23,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L23" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J23" s="5" t="str">
+        <f>IF(EXACT(I23,E23),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K23" s="4">
+        <f>ROW(A23)</f>
+        <v>23</v>
+      </c>
+      <c r="L23" s="4">
+        <f>IF(C23=C22,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M23" s="4">
-        <f t="shared" si="2"/>
-        <v>23</v>
+        <f>IF(C23=C24,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N23" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O23" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P23" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3072,42 +3016,40 @@
         <v>12</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K24" s="4" t="str">
+      <c r="H24" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A24,"0")," - ","CCMA - ",YEAR(F24)&amp;TEXT(MONTH(F24),"00")," - ",SUBSTITUTE(D24,"-","")," - ",B24)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I24" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C24,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L24" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J24" s="5" t="str">
+        <f>IF(EXACT(I24,E24),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K24" s="4">
+        <f>ROW(A24)</f>
+        <v>24</v>
+      </c>
+      <c r="L24" s="4">
+        <f>IF(C24=C23,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M24" s="4">
-        <f t="shared" si="2"/>
-        <v>24</v>
+        <f>IF(C24=C25,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N24" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O24" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P24" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3125,42 +3067,40 @@
         <v>12</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K25" s="4" t="str">
+      <c r="H25" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A25,"0")," - ","CCMA - ",YEAR(F25)&amp;TEXT(MONTH(F25),"00")," - ",SUBSTITUTE(D25,"-","")," - ",B25)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I25" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C25,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L25" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J25" s="5" t="str">
+        <f>IF(EXACT(I25,E25),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K25" s="4">
+        <f>ROW(A25)</f>
+        <v>25</v>
+      </c>
+      <c r="L25" s="4">
+        <f>IF(C25=C24,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M25" s="4">
-        <f t="shared" si="2"/>
-        <v>25</v>
+        <f>IF(C25=C26,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N25" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O25" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P25" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3178,42 +3118,40 @@
         <v>12</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K26" s="4" t="str">
+      <c r="H26" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A26,"0")," - ","CCMA - ",YEAR(F26)&amp;TEXT(MONTH(F26),"00")," - ",SUBSTITUTE(D26,"-","")," - ",B26)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I26" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C26,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L26" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J26" s="5" t="str">
+        <f>IF(EXACT(I26,E26),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K26" s="4">
+        <f>ROW(A26)</f>
+        <v>26</v>
+      </c>
+      <c r="L26" s="4">
+        <f>IF(C26=C25,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M26" s="4">
-        <f t="shared" si="2"/>
-        <v>26</v>
+        <f>IF(C26=C27,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N26" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O26" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P26" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3231,42 +3169,40 @@
         <v>12</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K27" s="4" t="str">
+      <c r="H27" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A27,"0")," - ","CCMA - ",YEAR(F27)&amp;TEXT(MONTH(F27),"00")," - ",SUBSTITUTE(D27,"-","")," - ",B27)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I27" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C27,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L27" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J27" s="5" t="str">
+        <f>IF(EXACT(I27,E27),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K27" s="4">
+        <f>ROW(A27)</f>
+        <v>27</v>
+      </c>
+      <c r="L27" s="4">
+        <f>IF(C27=C26,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M27" s="4">
-        <f t="shared" si="2"/>
-        <v>27</v>
+        <f>IF(C27=C28,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N27" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O27" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P27" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3284,42 +3220,40 @@
         <v>12</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K28" s="4" t="str">
+      <c r="H28" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A28,"0")," - ","CCMA - ",YEAR(F28)&amp;TEXT(MONTH(F28),"00")," - ",SUBSTITUTE(D28,"-","")," - ",B28)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I28" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C28,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L28" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J28" s="5" t="str">
+        <f>IF(EXACT(I28,E28),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K28" s="4">
+        <f>ROW(A28)</f>
+        <v>28</v>
+      </c>
+      <c r="L28" s="4">
+        <f>IF(C28=C27,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M28" s="4">
-        <f t="shared" si="2"/>
-        <v>28</v>
+        <f>IF(C28=C29,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N28" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O28" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P28" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3337,42 +3271,40 @@
         <v>12</v>
       </c>
       <c r="F29" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K29" s="4" t="str">
+      <c r="H29" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A29,"0")," - ","CCMA - ",YEAR(F29)&amp;TEXT(MONTH(F29),"00")," - ",SUBSTITUTE(D29,"-","")," - ",B29)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I29" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C29,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L29" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J29" s="5" t="str">
+        <f>IF(EXACT(I29,E29),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K29" s="4">
+        <f>ROW(A29)</f>
+        <v>29</v>
+      </c>
+      <c r="L29" s="4">
+        <f>IF(C29=C28,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M29" s="4">
-        <f t="shared" si="2"/>
-        <v>29</v>
+        <f>IF(C29=C30,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N29" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O29" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P29" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3390,42 +3322,40 @@
         <v>12</v>
       </c>
       <c r="F30" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K30" s="4" t="str">
+      <c r="H30" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A30,"0")," - ","CCMA - ",YEAR(F30)&amp;TEXT(MONTH(F30),"00")," - ",SUBSTITUTE(D30,"-","")," - ",B30)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I30" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C30,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L30" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J30" s="5" t="str">
+        <f>IF(EXACT(I30,E30),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K30" s="4">
+        <f>ROW(A30)</f>
+        <v>30</v>
+      </c>
+      <c r="L30" s="4">
+        <f>IF(C30=C29,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M30" s="4">
-        <f t="shared" si="2"/>
-        <v>30</v>
+        <f>IF(C30=C31,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N30" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O30" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P30" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3443,42 +3373,40 @@
         <v>12</v>
       </c>
       <c r="F31" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K31" s="4" t="str">
+      <c r="H31" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A31,"0")," - ","CCMA - ",YEAR(F31)&amp;TEXT(MONTH(F31),"00")," - ",SUBSTITUTE(D31,"-","")," - ",B31)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I31" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C31,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L31" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J31" s="5" t="str">
+        <f>IF(EXACT(I31,E31),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K31" s="4">
+        <f>ROW(A31)</f>
+        <v>31</v>
+      </c>
+      <c r="L31" s="4">
+        <f>IF(C31=C30,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M31" s="4">
-        <f t="shared" si="2"/>
-        <v>31</v>
+        <f>IF(C31=C32,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N31" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O31" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P31" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3496,42 +3424,40 @@
         <v>12</v>
       </c>
       <c r="F32" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K32" s="4" t="str">
+      <c r="H32" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A32,"0")," - ","CCMA - ",YEAR(F32)&amp;TEXT(MONTH(F32),"00")," - ",SUBSTITUTE(D32,"-","")," - ",B32)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I32" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C32,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L32" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J32" s="5" t="str">
+        <f>IF(EXACT(I32,E32),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K32" s="4">
+        <f>ROW(A32)</f>
+        <v>32</v>
+      </c>
+      <c r="L32" s="4">
+        <f>IF(C32=C31,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M32" s="4">
-        <f t="shared" si="2"/>
-        <v>32</v>
+        <f>IF(C32=C33,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N32" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O32" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P32" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3549,44 +3475,42 @@
         <v>12</v>
       </c>
       <c r="F33" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K33" s="4" t="str">
+      <c r="H33" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A33,"0")," - ","CCMA - ",YEAR(F33)&amp;TEXT(MONTH(F33),"00")," - ",SUBSTITUTE(D33,"-","")," - ",B33)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I33" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C33,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L33" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>x</v>
+      <c r="J33" s="5" t="str">
+        <f>IF(EXACT(I33,E33),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K33" s="4">
+        <f>ROW(A33)</f>
+        <v>33</v>
+      </c>
+      <c r="L33" s="4">
+        <f>IF(C33=C32,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M33" s="4">
-        <f t="shared" si="2"/>
-        <v>33</v>
+        <f>IF(C33=C34,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N33" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O33" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P33" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="str">
-        <f t="shared" ref="A34:A69" si="11">RIGHT(D34,1)</f>
+        <f t="shared" ref="A34:A69" si="4">RIGHT(D34,1)</f>
         <v>0</v>
       </c>
       <c r="B34" t="s">
@@ -3602,44 +3526,42 @@
         <v>12</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K34" s="4" t="str">
+      <c r="H34" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A34,"0")," - ","CCMA - ",YEAR(F34)&amp;TEXT(MONTH(F34),"00")," - ",SUBSTITUTE(D34,"-","")," - ",B34)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I34" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C34,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L34" s="5" t="str">
-        <f t="shared" ref="L34:L65" si="12">IF(EXACT(K34,E34),"ü","x")</f>
-        <v>x</v>
+      <c r="J34" s="5" t="str">
+        <f>IF(EXACT(I34,E34),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K34" s="4">
+        <f>ROW(A34)</f>
+        <v>34</v>
+      </c>
+      <c r="L34" s="4">
+        <f>IF(C34=C33,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M34" s="4">
-        <f t="shared" ref="M34:M69" si="13">ROW(A34)</f>
-        <v>34</v>
+        <f>IF(C34=C35,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N34" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O34" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P34" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B35" t="s">
@@ -3655,44 +3577,42 @@
         <v>12</v>
       </c>
       <c r="F35" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K35" s="4" t="str">
+      <c r="H35" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A35,"0")," - ","CCMA - ",YEAR(F35)&amp;TEXT(MONTH(F35),"00")," - ",SUBSTITUTE(D35,"-","")," - ",B35)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I35" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C35,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L35" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J35" s="5" t="str">
+        <f>IF(EXACT(I35,E35),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K35" s="4">
+        <f>ROW(A35)</f>
+        <v>35</v>
+      </c>
+      <c r="L35" s="4">
+        <f>IF(C35=C34,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M35" s="4">
-        <f t="shared" si="13"/>
-        <v>35</v>
+        <f>IF(C35=C36,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N35" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O35" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P35" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B36" t="s">
@@ -3708,44 +3628,42 @@
         <v>12</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K36" s="4" t="str">
+      <c r="H36" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A36,"0")," - ","CCMA - ",YEAR(F36)&amp;TEXT(MONTH(F36),"00")," - ",SUBSTITUTE(D36,"-","")," - ",B36)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I36" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C36,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L36" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J36" s="5" t="str">
+        <f>IF(EXACT(I36,E36),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K36" s="4">
+        <f>ROW(A36)</f>
+        <v>36</v>
+      </c>
+      <c r="L36" s="4">
+        <f>IF(C36=C35,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M36" s="4">
-        <f t="shared" si="13"/>
-        <v>36</v>
+        <f>IF(C36=C37,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N36" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O36" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P36" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B37" t="s">
@@ -3761,44 +3679,42 @@
         <v>12</v>
       </c>
       <c r="F37" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K37" s="4" t="str">
+      <c r="H37" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A37,"0")," - ","CCMA - ",YEAR(F37)&amp;TEXT(MONTH(F37),"00")," - ",SUBSTITUTE(D37,"-","")," - ",B37)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I37" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C37,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L37" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J37" s="5" t="str">
+        <f>IF(EXACT(I37,E37),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K37" s="4">
+        <f>ROW(A37)</f>
+        <v>37</v>
+      </c>
+      <c r="L37" s="4">
+        <f>IF(C37=C36,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M37" s="4">
-        <f t="shared" si="13"/>
-        <v>37</v>
+        <f>IF(C37=C38,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N37" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O37" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P37" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B38" t="s">
@@ -3814,44 +3730,42 @@
         <v>12</v>
       </c>
       <c r="F38" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K38" s="4" t="str">
+      <c r="H38" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A38,"0")," - ","CCMA - ",YEAR(F38)&amp;TEXT(MONTH(F38),"00")," - ",SUBSTITUTE(D38,"-","")," - ",B38)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I38" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C38,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L38" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J38" s="5" t="str">
+        <f>IF(EXACT(I38,E38),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K38" s="4">
+        <f>ROW(A38)</f>
+        <v>38</v>
+      </c>
+      <c r="L38" s="4">
+        <f>IF(C38=C37,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M38" s="4">
-        <f t="shared" si="13"/>
-        <v>38</v>
+        <f>IF(C38=C39,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N38" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O38" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P38" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B39" t="s">
@@ -3867,44 +3781,42 @@
         <v>12</v>
       </c>
       <c r="F39" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K39" s="4" t="str">
+      <c r="H39" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A39,"0")," - ","CCMA - ",YEAR(F39)&amp;TEXT(MONTH(F39),"00")," - ",SUBSTITUTE(D39,"-","")," - ",B39)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I39" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C39,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L39" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J39" s="5" t="str">
+        <f>IF(EXACT(I39,E39),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K39" s="4">
+        <f>ROW(A39)</f>
+        <v>39</v>
+      </c>
+      <c r="L39" s="4">
+        <f>IF(C39=C38,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M39" s="4">
-        <f t="shared" si="13"/>
-        <v>39</v>
+        <f>IF(C39=C40,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N39" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O39" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P39" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B40" t="s">
@@ -3920,44 +3832,42 @@
         <v>12</v>
       </c>
       <c r="F40" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K40" s="4" t="str">
+      <c r="H40" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A40,"0")," - ","CCMA - ",YEAR(F40)&amp;TEXT(MONTH(F40),"00")," - ",SUBSTITUTE(D40,"-","")," - ",B40)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I40" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C40,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L40" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J40" s="5" t="str">
+        <f>IF(EXACT(I40,E40),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K40" s="4">
+        <f>ROW(A40)</f>
+        <v>40</v>
+      </c>
+      <c r="L40" s="4">
+        <f>IF(C40=C39,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M40" s="4">
-        <f t="shared" si="13"/>
-        <v>40</v>
+        <f>IF(C40=C41,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N40" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O40" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P40" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B41" t="s">
@@ -3973,44 +3883,42 @@
         <v>12</v>
       </c>
       <c r="F41" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K41" s="4" t="str">
+      <c r="H41" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A41,"0")," - ","CCMA - ",YEAR(F41)&amp;TEXT(MONTH(F41),"00")," - ",SUBSTITUTE(D41,"-","")," - ",B41)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I41" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C41,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L41" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J41" s="5" t="str">
+        <f>IF(EXACT(I41,E41),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K41" s="4">
+        <f>ROW(A41)</f>
+        <v>41</v>
+      </c>
+      <c r="L41" s="4">
+        <f>IF(C41=C40,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M41" s="4">
-        <f t="shared" si="13"/>
-        <v>41</v>
+        <f>IF(C41=C42,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N41" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O41" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P41" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B42" t="s">
@@ -4026,44 +3934,42 @@
         <v>12</v>
       </c>
       <c r="F42" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K42" s="4" t="str">
+      <c r="H42" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A42,"0")," - ","CCMA - ",YEAR(F42)&amp;TEXT(MONTH(F42),"00")," - ",SUBSTITUTE(D42,"-","")," - ",B42)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I42" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C42,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L42" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J42" s="5" t="str">
+        <f>IF(EXACT(I42,E42),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K42" s="4">
+        <f>ROW(A42)</f>
+        <v>42</v>
+      </c>
+      <c r="L42" s="4">
+        <f>IF(C42=C41,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M42" s="4">
-        <f t="shared" si="13"/>
-        <v>42</v>
+        <f>IF(C42=C43,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N42" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O42" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P42" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B43" t="s">
@@ -4079,44 +3985,42 @@
         <v>12</v>
       </c>
       <c r="F43" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K43" s="4" t="str">
+      <c r="H43" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A43,"0")," - ","CCMA - ",YEAR(F43)&amp;TEXT(MONTH(F43),"00")," - ",SUBSTITUTE(D43,"-","")," - ",B43)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I43" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C43,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L43" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J43" s="5" t="str">
+        <f>IF(EXACT(I43,E43),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K43" s="4">
+        <f>ROW(A43)</f>
+        <v>43</v>
+      </c>
+      <c r="L43" s="4">
+        <f>IF(C43=C42,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M43" s="4">
-        <f t="shared" si="13"/>
-        <v>43</v>
+        <f>IF(C43=C44,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N43" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O43" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P43" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B44" t="s">
@@ -4132,44 +4036,42 @@
         <v>12</v>
       </c>
       <c r="F44" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K44" s="4" t="str">
+      <c r="H44" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A44,"0")," - ","CCMA - ",YEAR(F44)&amp;TEXT(MONTH(F44),"00")," - ",SUBSTITUTE(D44,"-","")," - ",B44)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I44" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C44,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L44" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J44" s="5" t="str">
+        <f>IF(EXACT(I44,E44),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K44" s="4">
+        <f>ROW(A44)</f>
+        <v>44</v>
+      </c>
+      <c r="L44" s="4">
+        <f>IF(C44=C43,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M44" s="4">
-        <f t="shared" si="13"/>
-        <v>44</v>
+        <f>IF(C44=C45,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N44" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O44" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P44" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B45" t="s">
@@ -4185,44 +4087,42 @@
         <v>12</v>
       </c>
       <c r="F45" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K45" s="4" t="str">
+      <c r="H45" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A45,"0")," - ","CCMA - ",YEAR(F45)&amp;TEXT(MONTH(F45),"00")," - ",SUBSTITUTE(D45,"-","")," - ",B45)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I45" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C45,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L45" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J45" s="5" t="str">
+        <f>IF(EXACT(I45,E45),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K45" s="4">
+        <f>ROW(A45)</f>
+        <v>45</v>
+      </c>
+      <c r="L45" s="4">
+        <f>IF(C45=C44,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M45" s="4">
-        <f t="shared" si="13"/>
-        <v>45</v>
+        <f>IF(C45=C46,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N45" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O45" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P45" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B46" t="s">
@@ -4238,44 +4138,42 @@
         <v>12</v>
       </c>
       <c r="F46" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K46" s="4" t="str">
+      <c r="H46" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A46,"0")," - ","CCMA - ",YEAR(F46)&amp;TEXT(MONTH(F46),"00")," - ",SUBSTITUTE(D46,"-","")," - ",B46)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I46" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C46,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L46" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J46" s="5" t="str">
+        <f>IF(EXACT(I46,E46),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K46" s="4">
+        <f>ROW(A46)</f>
+        <v>46</v>
+      </c>
+      <c r="L46" s="4">
+        <f>IF(C46=C45,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M46" s="4">
-        <f t="shared" si="13"/>
-        <v>46</v>
+        <f>IF(C46=C47,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N46" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O46" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P46" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B47" t="s">
@@ -4291,44 +4189,42 @@
         <v>12</v>
       </c>
       <c r="F47" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K47" s="4" t="str">
+      <c r="H47" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A47,"0")," - ","CCMA - ",YEAR(F47)&amp;TEXT(MONTH(F47),"00")," - ",SUBSTITUTE(D47,"-","")," - ",B47)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I47" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C47,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L47" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J47" s="5" t="str">
+        <f>IF(EXACT(I47,E47),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K47" s="4">
+        <f>ROW(A47)</f>
+        <v>47</v>
+      </c>
+      <c r="L47" s="4">
+        <f>IF(C47=C46,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M47" s="4">
-        <f t="shared" si="13"/>
-        <v>47</v>
+        <f>IF(C47=C48,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N47" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O47" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P47" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B48" t="s">
@@ -4344,44 +4240,42 @@
         <v>12</v>
       </c>
       <c r="F48" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K48" s="4" t="str">
+      <c r="H48" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A48,"0")," - ","CCMA - ",YEAR(F48)&amp;TEXT(MONTH(F48),"00")," - ",SUBSTITUTE(D48,"-","")," - ",B48)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I48" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C48,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L48" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J48" s="5" t="str">
+        <f>IF(EXACT(I48,E48),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K48" s="4">
+        <f>ROW(A48)</f>
+        <v>48</v>
+      </c>
+      <c r="L48" s="4">
+        <f>IF(C48=C47,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M48" s="4">
-        <f t="shared" si="13"/>
-        <v>48</v>
+        <f>IF(C48=C49,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N48" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O48" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P48" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B49" t="s">
@@ -4397,44 +4291,42 @@
         <v>12</v>
       </c>
       <c r="F49" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K49" s="4" t="str">
+      <c r="H49" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A49,"0")," - ","CCMA - ",YEAR(F49)&amp;TEXT(MONTH(F49),"00")," - ",SUBSTITUTE(D49,"-","")," - ",B49)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I49" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C49,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L49" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J49" s="5" t="str">
+        <f>IF(EXACT(I49,E49),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K49" s="4">
+        <f>ROW(A49)</f>
+        <v>49</v>
+      </c>
+      <c r="L49" s="4">
+        <f>IF(C49=C48,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M49" s="4">
-        <f t="shared" si="13"/>
-        <v>49</v>
+        <f>IF(C49=C50,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N49" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O49" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P49" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B50" t="s">
@@ -4450,44 +4342,42 @@
         <v>12</v>
       </c>
       <c r="F50" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K50" s="4" t="str">
+      <c r="H50" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A50,"0")," - ","CCMA - ",YEAR(F50)&amp;TEXT(MONTH(F50),"00")," - ",SUBSTITUTE(D50,"-","")," - ",B50)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I50" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C50,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L50" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J50" s="5" t="str">
+        <f>IF(EXACT(I50,E50),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K50" s="4">
+        <f>ROW(A50)</f>
+        <v>50</v>
+      </c>
+      <c r="L50" s="4">
+        <f>IF(C50=C49,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M50" s="4">
-        <f t="shared" si="13"/>
-        <v>50</v>
+        <f>IF(C50=C51,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N50" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O50" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P50" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B51" t="s">
@@ -4503,44 +4393,42 @@
         <v>12</v>
       </c>
       <c r="F51" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K51" s="4" t="str">
+      <c r="H51" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A51,"0")," - ","CCMA - ",YEAR(F51)&amp;TEXT(MONTH(F51),"00")," - ",SUBSTITUTE(D51,"-","")," - ",B51)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I51" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C51,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L51" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J51" s="5" t="str">
+        <f>IF(EXACT(I51,E51),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K51" s="4">
+        <f>ROW(A51)</f>
+        <v>51</v>
+      </c>
+      <c r="L51" s="4">
+        <f>IF(C51=C50,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M51" s="4">
-        <f t="shared" si="13"/>
-        <v>51</v>
+        <f>IF(C51=C52,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N51" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O51" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P51" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B52" t="s">
@@ -4556,44 +4444,42 @@
         <v>12</v>
       </c>
       <c r="F52" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K52" s="4" t="str">
+      <c r="H52" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A52,"0")," - ","CCMA - ",YEAR(F52)&amp;TEXT(MONTH(F52),"00")," - ",SUBSTITUTE(D52,"-","")," - ",B52)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I52" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C52,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L52" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J52" s="5" t="str">
+        <f>IF(EXACT(I52,E52),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K52" s="4">
+        <f>ROW(A52)</f>
+        <v>52</v>
+      </c>
+      <c r="L52" s="4">
+        <f>IF(C52=C51,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M52" s="4">
-        <f t="shared" si="13"/>
-        <v>52</v>
+        <f>IF(C52=C53,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N52" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O52" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P52" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B53" t="s">
@@ -4609,44 +4495,42 @@
         <v>12</v>
       </c>
       <c r="F53" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K53" s="4" t="str">
+      <c r="H53" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A53,"0")," - ","CCMA - ",YEAR(F53)&amp;TEXT(MONTH(F53),"00")," - ",SUBSTITUTE(D53,"-","")," - ",B53)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I53" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C53,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L53" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J53" s="5" t="str">
+        <f>IF(EXACT(I53,E53),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K53" s="4">
+        <f>ROW(A53)</f>
+        <v>53</v>
+      </c>
+      <c r="L53" s="4">
+        <f>IF(C53=C52,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M53" s="4">
-        <f t="shared" si="13"/>
-        <v>53</v>
+        <f>IF(C53=C54,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N53" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O53" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P53" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B54" t="s">
@@ -4662,44 +4546,42 @@
         <v>12</v>
       </c>
       <c r="F54" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K54" s="4" t="str">
+      <c r="H54" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A54,"0")," - ","CCMA - ",YEAR(F54)&amp;TEXT(MONTH(F54),"00")," - ",SUBSTITUTE(D54,"-","")," - ",B54)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I54" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C54,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L54" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J54" s="5" t="str">
+        <f>IF(EXACT(I54,E54),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K54" s="4">
+        <f>ROW(A54)</f>
+        <v>54</v>
+      </c>
+      <c r="L54" s="4">
+        <f>IF(C54=C53,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M54" s="4">
-        <f t="shared" si="13"/>
-        <v>54</v>
+        <f>IF(C54=C55,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N54" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O54" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P54" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B55" t="s">
@@ -4715,44 +4597,42 @@
         <v>12</v>
       </c>
       <c r="F55" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K55" s="4" t="str">
+      <c r="H55" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A55,"0")," - ","CCMA - ",YEAR(F55)&amp;TEXT(MONTH(F55),"00")," - ",SUBSTITUTE(D55,"-","")," - ",B55)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I55" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C55,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L55" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J55" s="5" t="str">
+        <f>IF(EXACT(I55,E55),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K55" s="4">
+        <f>ROW(A55)</f>
+        <v>55</v>
+      </c>
+      <c r="L55" s="4">
+        <f>IF(C55=C54,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M55" s="4">
-        <f t="shared" si="13"/>
-        <v>55</v>
+        <f>IF(C55=C56,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N55" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O55" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P55" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B56" t="s">
@@ -4768,44 +4648,42 @@
         <v>12</v>
       </c>
       <c r="F56" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K56" s="4" t="str">
+      <c r="H56" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A56,"0")," - ","CCMA - ",YEAR(F56)&amp;TEXT(MONTH(F56),"00")," - ",SUBSTITUTE(D56,"-","")," - ",B56)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I56" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C56,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L56" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J56" s="5" t="str">
+        <f>IF(EXACT(I56,E56),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K56" s="4">
+        <f>ROW(A56)</f>
+        <v>56</v>
+      </c>
+      <c r="L56" s="4">
+        <f>IF(C56=C55,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M56" s="4">
-        <f t="shared" si="13"/>
-        <v>56</v>
+        <f>IF(C56=C57,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N56" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O56" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P56" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B57" t="s">
@@ -4821,44 +4699,42 @@
         <v>12</v>
       </c>
       <c r="F57" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K57" s="4" t="str">
+      <c r="H57" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A57,"0")," - ","CCMA - ",YEAR(F57)&amp;TEXT(MONTH(F57),"00")," - ",SUBSTITUTE(D57,"-","")," - ",B57)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I57" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C57,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L57" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J57" s="5" t="str">
+        <f>IF(EXACT(I57,E57),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K57" s="4">
+        <f>ROW(A57)</f>
+        <v>57</v>
+      </c>
+      <c r="L57" s="4">
+        <f>IF(C57=C56,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M57" s="4">
-        <f t="shared" si="13"/>
-        <v>57</v>
+        <f>IF(C57=C58,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N57" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O57" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P57" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B58" t="s">
@@ -4874,44 +4750,42 @@
         <v>12</v>
       </c>
       <c r="F58" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K58" s="4" t="str">
+      <c r="H58" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A58,"0")," - ","CCMA - ",YEAR(F58)&amp;TEXT(MONTH(F58),"00")," - ",SUBSTITUTE(D58,"-","")," - ",B58)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I58" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C58,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L58" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J58" s="5" t="str">
+        <f>IF(EXACT(I58,E58),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K58" s="4">
+        <f>ROW(A58)</f>
+        <v>58</v>
+      </c>
+      <c r="L58" s="4">
+        <f>IF(C58=C57,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M58" s="4">
-        <f t="shared" si="13"/>
-        <v>58</v>
+        <f>IF(C58=C59,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N58" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O58" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P58" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B59" t="s">
@@ -4927,44 +4801,42 @@
         <v>12</v>
       </c>
       <c r="F59" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="3"/>
-      <c r="J59" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K59" s="4" t="str">
+      <c r="H59" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A59,"0")," - ","CCMA - ",YEAR(F59)&amp;TEXT(MONTH(F59),"00")," - ",SUBSTITUTE(D59,"-","")," - ",B59)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I59" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C59,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L59" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J59" s="5" t="str">
+        <f>IF(EXACT(I59,E59),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K59" s="4">
+        <f>ROW(A59)</f>
+        <v>59</v>
+      </c>
+      <c r="L59" s="4">
+        <f>IF(C59=C58,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M59" s="4">
-        <f t="shared" si="13"/>
-        <v>59</v>
+        <f>IF(C59=C60,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N59" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O59" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P59" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B60" t="s">
@@ -4980,44 +4852,42 @@
         <v>12</v>
       </c>
       <c r="F60" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
-      <c r="J60" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K60" s="4" t="str">
+      <c r="H60" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A60,"0")," - ","CCMA - ",YEAR(F60)&amp;TEXT(MONTH(F60),"00")," - ",SUBSTITUTE(D60,"-","")," - ",B60)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I60" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C60,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L60" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J60" s="5" t="str">
+        <f>IF(EXACT(I60,E60),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K60" s="4">
+        <f>ROW(A60)</f>
+        <v>60</v>
+      </c>
+      <c r="L60" s="4">
+        <f>IF(C60=C59,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M60" s="4">
-        <f t="shared" si="13"/>
-        <v>60</v>
+        <f>IF(C60=C61,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N60" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O60" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P60" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B61" t="s">
@@ -5033,44 +4903,42 @@
         <v>12</v>
       </c>
       <c r="F61" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K61" s="4" t="str">
+      <c r="H61" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A61,"0")," - ","CCMA - ",YEAR(F61)&amp;TEXT(MONTH(F61),"00")," - ",SUBSTITUTE(D61,"-","")," - ",B61)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I61" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C61,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L61" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J61" s="5" t="str">
+        <f>IF(EXACT(I61,E61),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K61" s="4">
+        <f>ROW(A61)</f>
+        <v>61</v>
+      </c>
+      <c r="L61" s="4">
+        <f>IF(C61=C60,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M61" s="4">
-        <f t="shared" si="13"/>
-        <v>61</v>
+        <f>IF(C61=C62,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N61" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O61" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P61" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B62" t="s">
@@ -5086,44 +4954,42 @@
         <v>12</v>
       </c>
       <c r="F62" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K62" s="4" t="str">
+      <c r="H62" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A62,"0")," - ","CCMA - ",YEAR(F62)&amp;TEXT(MONTH(F62),"00")," - ",SUBSTITUTE(D62,"-","")," - ",B62)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I62" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C62,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L62" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J62" s="5" t="str">
+        <f>IF(EXACT(I62,E62),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K62" s="4">
+        <f>ROW(A62)</f>
+        <v>62</v>
+      </c>
+      <c r="L62" s="4">
+        <f>IF(C62=C61,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M62" s="4">
-        <f t="shared" si="13"/>
-        <v>62</v>
+        <f>IF(C62=C63,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N62" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O62" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P62" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B63" t="s">
@@ -5139,44 +5005,42 @@
         <v>12</v>
       </c>
       <c r="F63" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
-      <c r="J63" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K63" s="4" t="str">
+      <c r="H63" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A63,"0")," - ","CCMA - ",YEAR(F63)&amp;TEXT(MONTH(F63),"00")," - ",SUBSTITUTE(D63,"-","")," - ",B63)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I63" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C63,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L63" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J63" s="5" t="str">
+        <f>IF(EXACT(I63,E63),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K63" s="4">
+        <f>ROW(A63)</f>
+        <v>63</v>
+      </c>
+      <c r="L63" s="4">
+        <f>IF(C63=C62,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M63" s="4">
-        <f t="shared" si="13"/>
-        <v>63</v>
+        <f>IF(C63=C64,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N63" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O63" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P63" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B64" t="s">
@@ -5192,44 +5056,42 @@
         <v>12</v>
       </c>
       <c r="F64" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
-      <c r="J64" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K64" s="4" t="str">
+      <c r="H64" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A64,"0")," - ","CCMA - ",YEAR(F64)&amp;TEXT(MONTH(F64),"00")," - ",SUBSTITUTE(D64,"-","")," - ",B64)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I64" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C64,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L64" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J64" s="5" t="str">
+        <f>IF(EXACT(I64,E64),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K64" s="4">
+        <f>ROW(A64)</f>
+        <v>64</v>
+      </c>
+      <c r="L64" s="4">
+        <f>IF(C64=C63,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M64" s="4">
-        <f t="shared" si="13"/>
-        <v>64</v>
+        <f>IF(C64=C65,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N64" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O64" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P64" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B65" t="s">
@@ -5245,44 +5107,42 @@
         <v>12</v>
       </c>
       <c r="F65" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
-      <c r="J65" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K65" s="4" t="str">
+      <c r="H65" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A65,"0")," - ","CCMA - ",YEAR(F65)&amp;TEXT(MONTH(F65),"00")," - ",SUBSTITUTE(D65,"-","")," - ",B65)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I65" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C65,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L65" s="5" t="str">
-        <f t="shared" si="12"/>
-        <v>x</v>
+      <c r="J65" s="5" t="str">
+        <f>IF(EXACT(I65,E65),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K65" s="4">
+        <f>ROW(A65)</f>
+        <v>65</v>
+      </c>
+      <c r="L65" s="4">
+        <f>IF(C65=C64,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M65" s="4">
-        <f t="shared" si="13"/>
-        <v>65</v>
+        <f>IF(C65=C66,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N65" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O65" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P65" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B66" t="s">
@@ -5298,44 +5158,42 @@
         <v>12</v>
       </c>
       <c r="F66" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45131</v>
       </c>
       <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
-      <c r="J66" s="2" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K66" s="4" t="str">
+      <c r="H66" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A66,"0")," - ","CCMA - ",YEAR(F66)&amp;TEXT(MONTH(F66),"00")," - ",SUBSTITUTE(D66,"-","")," - ",B66)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I66" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C66,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L66" s="5" t="str">
-        <f t="shared" ref="L66:L69" si="14">IF(EXACT(K66,E66),"ü","x")</f>
-        <v>x</v>
+      <c r="J66" s="5" t="str">
+        <f>IF(EXACT(I66,E66),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K66" s="4">
+        <f>ROW(A66)</f>
+        <v>66</v>
+      </c>
+      <c r="L66" s="4">
+        <f>IF(C66=C65,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M66" s="4">
-        <f t="shared" si="13"/>
-        <v>66</v>
+        <f>IF(C66=C67,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N66" s="4">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O66" s="4">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P66" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B67" t="s">
@@ -5351,44 +5209,42 @@
         <v>12</v>
       </c>
       <c r="F67" s="3">
-        <f t="shared" ref="F67:F69" ca="1" si="15">TODAY()</f>
-        <v>45125</v>
+        <f t="shared" ref="F67:F69" ca="1" si="5">TODAY()</f>
+        <v>45131</v>
       </c>
       <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
-      <c r="J67" s="2" t="str">
-        <f t="shared" ref="J67:J69" ca="1" si="16">CONCATENATE(TEXT(A67,"0")," - ","CCMA - ",YEAR(F67)&amp;TEXT(MONTH(F67),"00")," - ",SUBSTITUTE(D67,"-","")," - ",B67)</f>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K67" s="4" t="str">
+      <c r="H67" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A67,"0")," - ","CCMA - ",YEAR(F67)&amp;TEXT(MONTH(F67),"00")," - ",SUBSTITUTE(D67,"-","")," - ",B67)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I67" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C67,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L67" s="5" t="str">
-        <f t="shared" si="14"/>
-        <v>x</v>
+      <c r="J67" s="5" t="str">
+        <f>IF(EXACT(I67,E67),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K67" s="4">
+        <f>ROW(A67)</f>
+        <v>67</v>
+      </c>
+      <c r="L67" s="4">
+        <f>IF(C67=C66,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M67" s="4">
-        <f t="shared" si="13"/>
-        <v>67</v>
+        <f>IF(C67=C68,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N67" s="4">
-        <f t="shared" ref="N67:N69" si="17">IF(C67=C66,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="O67" s="4">
-        <f t="shared" ref="O67:O69" si="18">IF(C67=C68,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="P67" s="4">
-        <f t="shared" ref="P67:P69" si="19">SUM(N67:O67)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" ref="N67:N69" si="6">SUM(L67:M67)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B68" t="s">
@@ -5404,44 +5260,42 @@
         <v>12</v>
       </c>
       <c r="F68" s="3">
-        <f t="shared" ca="1" si="15"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>45131</v>
       </c>
       <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
-      <c r="J68" s="2" t="str">
-        <f t="shared" ca="1" si="16"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K68" s="4" t="str">
+      <c r="H68" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A68,"0")," - ","CCMA - ",YEAR(F68)&amp;TEXT(MONTH(F68),"00")," - ",SUBSTITUTE(D68,"-","")," - ",B68)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I68" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C68,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L68" s="5" t="str">
-        <f t="shared" si="14"/>
-        <v>x</v>
+      <c r="J68" s="5" t="str">
+        <f>IF(EXACT(I68,E68),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K68" s="4">
+        <f>ROW(A68)</f>
+        <v>68</v>
+      </c>
+      <c r="L68" s="4">
+        <f>IF(C68=C67,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M68" s="4">
-        <f t="shared" si="13"/>
-        <v>68</v>
+        <f>IF(C68=C69,1,0)</f>
+        <v>1</v>
       </c>
       <c r="N68" s="4">
-        <f t="shared" si="17"/>
-        <v>1</v>
-      </c>
-      <c r="O68" s="4">
-        <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="P68" s="4">
-        <f t="shared" si="19"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="B69" t="s">
@@ -5457,44 +5311,42 @@
         <v>12</v>
       </c>
       <c r="F69" s="3">
-        <f t="shared" ca="1" si="15"/>
-        <v>45125</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>45131</v>
       </c>
       <c r="G69" s="3"/>
-      <c r="H69" s="3"/>
-      <c r="I69" s="3"/>
-      <c r="J69" s="2" t="str">
-        <f t="shared" ca="1" si="16"/>
-        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
-      </c>
-      <c r="K69" s="4" t="str">
+      <c r="H69" s="2" t="str">
+        <f ca="1">CONCATENATE(TEXT(A69,"0")," - ","CCMA - ",YEAR(F69)&amp;TEXT(MONTH(F69),"00")," - ",SUBSTITUTE(D69,"-","")," - ",B69)</f>
+        <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
+      </c>
+      <c r="I69" s="4" t="str">
         <f>_xlfn.IFNA(VLOOKUP(C69,[1]Hoja1!$J:$L,3,0),"")</f>
         <v/>
       </c>
-      <c r="L69" s="5" t="str">
-        <f t="shared" si="14"/>
-        <v>x</v>
+      <c r="J69" s="5" t="str">
+        <f>IF(EXACT(I69,E69),"ü","x")</f>
+        <v>x</v>
+      </c>
+      <c r="K69" s="4">
+        <f>ROW(A69)</f>
+        <v>69</v>
+      </c>
+      <c r="L69" s="4">
+        <f>IF(C69=C68,1,0)</f>
+        <v>1</v>
       </c>
       <c r="M69" s="4">
-        <f t="shared" si="13"/>
-        <v>69</v>
+        <f>IF(C69=C70,1,0)</f>
+        <v>0</v>
       </c>
       <c r="N69" s="4">
-        <f t="shared" si="17"/>
-        <v>1</v>
-      </c>
-      <c r="O69" s="4">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="P69" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P69" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M69">
+  <autoFilter ref="A1:N69" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K69">
     <sortCondition ref="A2:A69"/>
     <sortCondition ref="D2:D69"/>
   </sortState>

</xml_diff>

<commit_message>
Update Excel: Initial question
</commit_message>
<xml_diff>
--- a/CCMA.xlsx
+++ b/CCMA.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
-  <workbookPr/>
+  <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\Descarga_CCMA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\BOT-Descarga-CCMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80321D5C-3A25-470D-9167-493B2D089605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA424C37-4A40-4879-BA63-A533844E3A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1813,7 +1813,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1894,11 +1894,11 @@
       </c>
       <c r="F2" s="3">
         <f ca="1">TODAY()</f>
-        <v>45131</v>
+        <v>45132</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A2,"0")," - ","CCMA - ",YEAR(F2)&amp;TEXT(MONTH(F2),"00")," - ",SUBSTITUTE(D2,"-","")," - ",B2)</f>
+        <f t="shared" ref="H2:H33" ca="1" si="1">CONCATENATE(TEXT(A2,"0")," - ","CCMA - ",YEAR(F2)&amp;TEXT(MONTH(F2),"00")," - ",SUBSTITUTE(D2,"-","")," - ",B2)</f>
         <v>0 - CCMA - 202307 - 20000000000 - Cliente</v>
       </c>
       <c r="I2" s="4" t="str">
@@ -1906,23 +1906,23 @@
         <v/>
       </c>
       <c r="J2" s="5" t="str">
-        <f>IF(EXACT(I2,E2),"ü","x")</f>
+        <f t="shared" ref="J2:J33" si="2">IF(EXACT(I2,E2),"ü","x")</f>
         <v>x</v>
       </c>
       <c r="K2" s="4">
-        <f>ROW(A2)</f>
+        <f t="shared" ref="K2:K33" si="3">ROW(A2)</f>
         <v>2</v>
       </c>
       <c r="L2" s="4">
-        <f>IF(C2=C1,1,0)</f>
+        <f t="shared" ref="L2:L33" si="4">IF(C2=C1,1,0)</f>
         <v>0</v>
       </c>
       <c r="M2" s="4">
-        <f>IF(C2=C3,1,0)</f>
+        <f t="shared" ref="M2:M33" si="5">IF(C2=C3,1,0)</f>
         <v>1</v>
       </c>
       <c r="N2" s="4">
-        <f t="shared" ref="N2" si="1">SUM(L2:M2)</f>
+        <f t="shared" ref="N2" si="6">SUM(L2:M2)</f>
         <v>1</v>
       </c>
     </row>
@@ -1945,12 +1945,12 @@
         <v>12</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F66" ca="1" si="2">TODAY()</f>
-        <v>45131</v>
+        <f t="shared" ref="F3:F66" ca="1" si="7">TODAY()</f>
+        <v>45132</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A3,"0")," - ","CCMA - ",YEAR(F3)&amp;TEXT(MONTH(F3),"00")," - ",SUBSTITUTE(D3,"-","")," - ",B3)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 20000000000 - Cliente</v>
       </c>
       <c r="I3" s="4" t="str">
@@ -1958,23 +1958,23 @@
         <v/>
       </c>
       <c r="J3" s="5" t="str">
-        <f>IF(EXACT(I3,E3),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K3" s="4">
-        <f>ROW(A3)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="L3" s="4">
-        <f>IF(C3=C2,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M3" s="4">
-        <f>IF(C3=C4,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N3" s="4">
-        <f t="shared" ref="N3:N66" si="3">SUM(L3:M3)</f>
+        <f t="shared" ref="N3:N66" si="8">SUM(L3:M3)</f>
         <v>2</v>
       </c>
     </row>
@@ -1996,12 +1996,12 @@
         <v>12</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A4,"0")," - ","CCMA - ",YEAR(F4)&amp;TEXT(MONTH(F4),"00")," - ",SUBSTITUTE(D4,"-","")," - ",B4)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I4" s="4" t="str">
@@ -2009,23 +2009,23 @@
         <v/>
       </c>
       <c r="J4" s="5" t="str">
-        <f>IF(EXACT(I4,E4),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K4" s="4">
-        <f>ROW(A4)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="L4" s="4">
-        <f>IF(C4=C3,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M4" s="4">
-        <f>IF(C4=C5,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N4" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2047,12 +2047,12 @@
         <v>12</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A5,"0")," - ","CCMA - ",YEAR(F5)&amp;TEXT(MONTH(F5),"00")," - ",SUBSTITUTE(D5,"-","")," - ",B5)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I5" s="4" t="str">
@@ -2060,23 +2060,23 @@
         <v/>
       </c>
       <c r="J5" s="5" t="str">
-        <f>IF(EXACT(I5,E5),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K5" s="4">
-        <f>ROW(A5)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="L5" s="4">
-        <f>IF(C5=C4,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M5" s="4">
-        <f>IF(C5=C6,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2098,12 +2098,12 @@
         <v>12</v>
       </c>
       <c r="F6" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A6,"0")," - ","CCMA - ",YEAR(F6)&amp;TEXT(MONTH(F6),"00")," - ",SUBSTITUTE(D6,"-","")," - ",B6)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I6" s="4" t="str">
@@ -2111,23 +2111,23 @@
         <v/>
       </c>
       <c r="J6" s="5" t="str">
-        <f>IF(EXACT(I6,E6),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K6" s="4">
-        <f>ROW(A6)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="L6" s="4">
-        <f>IF(C6=C5,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M6" s="4">
-        <f>IF(C6=C7,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2149,12 +2149,12 @@
         <v>12</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A7,"0")," - ","CCMA - ",YEAR(F7)&amp;TEXT(MONTH(F7),"00")," - ",SUBSTITUTE(D7,"-","")," - ",B7)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I7" s="4" t="str">
@@ -2162,23 +2162,23 @@
         <v/>
       </c>
       <c r="J7" s="5" t="str">
-        <f>IF(EXACT(I7,E7),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K7" s="4">
-        <f>ROW(A7)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="L7" s="4">
-        <f>IF(C7=C6,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M7" s="4">
-        <f>IF(C7=C8,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2200,12 +2200,12 @@
         <v>12</v>
       </c>
       <c r="F8" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A8,"0")," - ","CCMA - ",YEAR(F8)&amp;TEXT(MONTH(F8),"00")," - ",SUBSTITUTE(D8,"-","")," - ",B8)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I8" s="4" t="str">
@@ -2213,23 +2213,23 @@
         <v/>
       </c>
       <c r="J8" s="5" t="str">
-        <f>IF(EXACT(I8,E8),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K8" s="4">
-        <f>ROW(A8)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="L8" s="4">
-        <f>IF(C8=C7,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M8" s="4">
-        <f>IF(C8=C9,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N8" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2251,12 +2251,12 @@
         <v>12</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A9,"0")," - ","CCMA - ",YEAR(F9)&amp;TEXT(MONTH(F9),"00")," - ",SUBSTITUTE(D9,"-","")," - ",B9)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I9" s="4" t="str">
@@ -2264,23 +2264,23 @@
         <v/>
       </c>
       <c r="J9" s="5" t="str">
-        <f>IF(EXACT(I9,E9),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K9" s="4">
-        <f>ROW(A9)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="L9" s="4">
-        <f>IF(C9=C8,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M9" s="4">
-        <f>IF(C9=C10,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N9" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2302,12 +2302,12 @@
         <v>12</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A10,"0")," - ","CCMA - ",YEAR(F10)&amp;TEXT(MONTH(F10),"00")," - ",SUBSTITUTE(D10,"-","")," - ",B10)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I10" s="4" t="str">
@@ -2315,23 +2315,23 @@
         <v/>
       </c>
       <c r="J10" s="5" t="str">
-        <f>IF(EXACT(I10,E10),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K10" s="4">
-        <f>ROW(A10)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="L10" s="4">
-        <f>IF(C10=C9,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M10" s="4">
-        <f>IF(C10=C11,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N10" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2353,12 +2353,12 @@
         <v>12</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A11,"0")," - ","CCMA - ",YEAR(F11)&amp;TEXT(MONTH(F11),"00")," - ",SUBSTITUTE(D11,"-","")," - ",B11)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I11" s="4" t="str">
@@ -2366,23 +2366,23 @@
         <v/>
       </c>
       <c r="J11" s="5" t="str">
-        <f>IF(EXACT(I11,E11),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K11" s="4">
-        <f>ROW(A11)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="L11" s="4">
-        <f>IF(C11=C10,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M11" s="4">
-        <f>IF(C11=C12,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2404,12 +2404,12 @@
         <v>12</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A12,"0")," - ","CCMA - ",YEAR(F12)&amp;TEXT(MONTH(F12),"00")," - ",SUBSTITUTE(D12,"-","")," - ",B12)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I12" s="4" t="str">
@@ -2417,23 +2417,23 @@
         <v/>
       </c>
       <c r="J12" s="5" t="str">
-        <f>IF(EXACT(I12,E12),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K12" s="4">
-        <f>ROW(A12)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="L12" s="4">
-        <f>IF(C12=C11,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M12" s="4">
-        <f>IF(C12=C13,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N12" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2455,12 +2455,12 @@
         <v>12</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A13,"0")," - ","CCMA - ",YEAR(F13)&amp;TEXT(MONTH(F13),"00")," - ",SUBSTITUTE(D13,"-","")," - ",B13)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I13" s="4" t="str">
@@ -2468,23 +2468,23 @@
         <v/>
       </c>
       <c r="J13" s="5" t="str">
-        <f>IF(EXACT(I13,E13),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K13" s="4">
-        <f>ROW(A13)</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="L13" s="4">
-        <f>IF(C13=C12,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M13" s="4">
-        <f>IF(C13=C14,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N13" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2506,12 +2506,12 @@
         <v>12</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A14,"0")," - ","CCMA - ",YEAR(F14)&amp;TEXT(MONTH(F14),"00")," - ",SUBSTITUTE(D14,"-","")," - ",B14)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I14" s="4" t="str">
@@ -2519,23 +2519,23 @@
         <v/>
       </c>
       <c r="J14" s="5" t="str">
-        <f>IF(EXACT(I14,E14),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K14" s="4">
-        <f>ROW(A14)</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="L14" s="4">
-        <f>IF(C14=C13,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M14" s="4">
-        <f>IF(C14=C15,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N14" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2557,12 +2557,12 @@
         <v>12</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A15,"0")," - ","CCMA - ",YEAR(F15)&amp;TEXT(MONTH(F15),"00")," - ",SUBSTITUTE(D15,"-","")," - ",B15)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I15" s="4" t="str">
@@ -2570,23 +2570,23 @@
         <v/>
       </c>
       <c r="J15" s="5" t="str">
-        <f>IF(EXACT(I15,E15),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K15" s="4">
-        <f>ROW(A15)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="L15" s="4">
-        <f>IF(C15=C14,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M15" s="4">
-        <f>IF(C15=C16,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N15" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2608,12 +2608,12 @@
         <v>12</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A16,"0")," - ","CCMA - ",YEAR(F16)&amp;TEXT(MONTH(F16),"00")," - ",SUBSTITUTE(D16,"-","")," - ",B16)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I16" s="4" t="str">
@@ -2621,23 +2621,23 @@
         <v/>
       </c>
       <c r="J16" s="5" t="str">
-        <f>IF(EXACT(I16,E16),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K16" s="4">
-        <f>ROW(A16)</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="L16" s="4">
-        <f>IF(C16=C15,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M16" s="4">
-        <f>IF(C16=C17,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N16" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2659,12 +2659,12 @@
         <v>12</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A17,"0")," - ","CCMA - ",YEAR(F17)&amp;TEXT(MONTH(F17),"00")," - ",SUBSTITUTE(D17,"-","")," - ",B17)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I17" s="4" t="str">
@@ -2672,23 +2672,23 @@
         <v/>
       </c>
       <c r="J17" s="5" t="str">
-        <f>IF(EXACT(I17,E17),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K17" s="4">
-        <f>ROW(A17)</f>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="L17" s="4">
-        <f>IF(C17=C16,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M17" s="4">
-        <f>IF(C17=C18,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N17" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2710,12 +2710,12 @@
         <v>12</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A18,"0")," - ","CCMA - ",YEAR(F18)&amp;TEXT(MONTH(F18),"00")," - ",SUBSTITUTE(D18,"-","")," - ",B18)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I18" s="4" t="str">
@@ -2723,23 +2723,23 @@
         <v/>
       </c>
       <c r="J18" s="5" t="str">
-        <f>IF(EXACT(I18,E18),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K18" s="4">
-        <f>ROW(A18)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="L18" s="4">
-        <f>IF(C18=C17,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M18" s="4">
-        <f>IF(C18=C19,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N18" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2761,12 +2761,12 @@
         <v>12</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A19,"0")," - ","CCMA - ",YEAR(F19)&amp;TEXT(MONTH(F19),"00")," - ",SUBSTITUTE(D19,"-","")," - ",B19)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I19" s="4" t="str">
@@ -2774,23 +2774,23 @@
         <v/>
       </c>
       <c r="J19" s="5" t="str">
-        <f>IF(EXACT(I19,E19),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K19" s="4">
-        <f>ROW(A19)</f>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="L19" s="4">
-        <f>IF(C19=C18,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M19" s="4">
-        <f>IF(C19=C20,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N19" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2812,12 +2812,12 @@
         <v>12</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A20,"0")," - ","CCMA - ",YEAR(F20)&amp;TEXT(MONTH(F20),"00")," - ",SUBSTITUTE(D20,"-","")," - ",B20)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I20" s="4" t="str">
@@ -2825,23 +2825,23 @@
         <v/>
       </c>
       <c r="J20" s="5" t="str">
-        <f>IF(EXACT(I20,E20),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K20" s="4">
-        <f>ROW(A20)</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="L20" s="4">
-        <f>IF(C20=C19,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M20" s="4">
-        <f>IF(C20=C21,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N20" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2863,12 +2863,12 @@
         <v>12</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A21,"0")," - ","CCMA - ",YEAR(F21)&amp;TEXT(MONTH(F21),"00")," - ",SUBSTITUTE(D21,"-","")," - ",B21)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I21" s="4" t="str">
@@ -2876,23 +2876,23 @@
         <v/>
       </c>
       <c r="J21" s="5" t="str">
-        <f>IF(EXACT(I21,E21),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K21" s="4">
-        <f>ROW(A21)</f>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="L21" s="4">
-        <f>IF(C21=C20,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M21" s="4">
-        <f>IF(C21=C22,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N21" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2914,12 +2914,12 @@
         <v>12</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A22,"0")," - ","CCMA - ",YEAR(F22)&amp;TEXT(MONTH(F22),"00")," - ",SUBSTITUTE(D22,"-","")," - ",B22)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I22" s="4" t="str">
@@ -2927,23 +2927,23 @@
         <v/>
       </c>
       <c r="J22" s="5" t="str">
-        <f>IF(EXACT(I22,E22),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K22" s="4">
-        <f>ROW(A22)</f>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="L22" s="4">
-        <f>IF(C22=C21,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M22" s="4">
-        <f>IF(C22=C23,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N22" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -2965,12 +2965,12 @@
         <v>12</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A23,"0")," - ","CCMA - ",YEAR(F23)&amp;TEXT(MONTH(F23),"00")," - ",SUBSTITUTE(D23,"-","")," - ",B23)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I23" s="4" t="str">
@@ -2978,23 +2978,23 @@
         <v/>
       </c>
       <c r="J23" s="5" t="str">
-        <f>IF(EXACT(I23,E23),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K23" s="4">
-        <f>ROW(A23)</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="L23" s="4">
-        <f>IF(C23=C22,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M23" s="4">
-        <f>IF(C23=C24,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N23" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -3016,12 +3016,12 @@
         <v>12</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A24,"0")," - ","CCMA - ",YEAR(F24)&amp;TEXT(MONTH(F24),"00")," - ",SUBSTITUTE(D24,"-","")," - ",B24)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I24" s="4" t="str">
@@ -3029,23 +3029,23 @@
         <v/>
       </c>
       <c r="J24" s="5" t="str">
-        <f>IF(EXACT(I24,E24),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K24" s="4">
-        <f>ROW(A24)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="L24" s="4">
-        <f>IF(C24=C23,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M24" s="4">
-        <f>IF(C24=C25,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N24" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -3067,12 +3067,12 @@
         <v>12</v>
       </c>
       <c r="F25" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A25,"0")," - ","CCMA - ",YEAR(F25)&amp;TEXT(MONTH(F25),"00")," - ",SUBSTITUTE(D25,"-","")," - ",B25)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I25" s="4" t="str">
@@ -3080,23 +3080,23 @@
         <v/>
       </c>
       <c r="J25" s="5" t="str">
-        <f>IF(EXACT(I25,E25),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K25" s="4">
-        <f>ROW(A25)</f>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="L25" s="4">
-        <f>IF(C25=C24,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M25" s="4">
-        <f>IF(C25=C26,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N25" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -3118,12 +3118,12 @@
         <v>12</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A26,"0")," - ","CCMA - ",YEAR(F26)&amp;TEXT(MONTH(F26),"00")," - ",SUBSTITUTE(D26,"-","")," - ",B26)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I26" s="4" t="str">
@@ -3131,23 +3131,23 @@
         <v/>
       </c>
       <c r="J26" s="5" t="str">
-        <f>IF(EXACT(I26,E26),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K26" s="4">
-        <f>ROW(A26)</f>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="L26" s="4">
-        <f>IF(C26=C25,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M26" s="4">
-        <f>IF(C26=C27,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N26" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -3169,12 +3169,12 @@
         <v>12</v>
       </c>
       <c r="F27" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A27,"0")," - ","CCMA - ",YEAR(F27)&amp;TEXT(MONTH(F27),"00")," - ",SUBSTITUTE(D27,"-","")," - ",B27)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I27" s="4" t="str">
@@ -3182,23 +3182,23 @@
         <v/>
       </c>
       <c r="J27" s="5" t="str">
-        <f>IF(EXACT(I27,E27),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K27" s="4">
-        <f>ROW(A27)</f>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="L27" s="4">
-        <f>IF(C27=C26,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M27" s="4">
-        <f>IF(C27=C28,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N27" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -3220,12 +3220,12 @@
         <v>12</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A28,"0")," - ","CCMA - ",YEAR(F28)&amp;TEXT(MONTH(F28),"00")," - ",SUBSTITUTE(D28,"-","")," - ",B28)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I28" s="4" t="str">
@@ -3233,23 +3233,23 @@
         <v/>
       </c>
       <c r="J28" s="5" t="str">
-        <f>IF(EXACT(I28,E28),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K28" s="4">
-        <f>ROW(A28)</f>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="L28" s="4">
-        <f>IF(C28=C27,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M28" s="4">
-        <f>IF(C28=C29,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N28" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -3271,12 +3271,12 @@
         <v>12</v>
       </c>
       <c r="F29" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A29,"0")," - ","CCMA - ",YEAR(F29)&amp;TEXT(MONTH(F29),"00")," - ",SUBSTITUTE(D29,"-","")," - ",B29)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I29" s="4" t="str">
@@ -3284,23 +3284,23 @@
         <v/>
       </c>
       <c r="J29" s="5" t="str">
-        <f>IF(EXACT(I29,E29),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K29" s="4">
-        <f>ROW(A29)</f>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="L29" s="4">
-        <f>IF(C29=C28,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M29" s="4">
-        <f>IF(C29=C30,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N29" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -3322,12 +3322,12 @@
         <v>12</v>
       </c>
       <c r="F30" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A30,"0")," - ","CCMA - ",YEAR(F30)&amp;TEXT(MONTH(F30),"00")," - ",SUBSTITUTE(D30,"-","")," - ",B30)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I30" s="4" t="str">
@@ -3335,23 +3335,23 @@
         <v/>
       </c>
       <c r="J30" s="5" t="str">
-        <f>IF(EXACT(I30,E30),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K30" s="4">
-        <f>ROW(A30)</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="L30" s="4">
-        <f>IF(C30=C29,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M30" s="4">
-        <f>IF(C30=C31,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N30" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -3373,12 +3373,12 @@
         <v>12</v>
       </c>
       <c r="F31" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A31,"0")," - ","CCMA - ",YEAR(F31)&amp;TEXT(MONTH(F31),"00")," - ",SUBSTITUTE(D31,"-","")," - ",B31)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I31" s="4" t="str">
@@ -3386,23 +3386,23 @@
         <v/>
       </c>
       <c r="J31" s="5" t="str">
-        <f>IF(EXACT(I31,E31),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K31" s="4">
-        <f>ROW(A31)</f>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="L31" s="4">
-        <f>IF(C31=C30,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M31" s="4">
-        <f>IF(C31=C32,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N31" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -3424,12 +3424,12 @@
         <v>12</v>
       </c>
       <c r="F32" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A32,"0")," - ","CCMA - ",YEAR(F32)&amp;TEXT(MONTH(F32),"00")," - ",SUBSTITUTE(D32,"-","")," - ",B32)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I32" s="4" t="str">
@@ -3437,23 +3437,23 @@
         <v/>
       </c>
       <c r="J32" s="5" t="str">
-        <f>IF(EXACT(I32,E32),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K32" s="4">
-        <f>ROW(A32)</f>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="L32" s="4">
-        <f>IF(C32=C31,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M32" s="4">
-        <f>IF(C32=C33,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N32" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -3475,12 +3475,12 @@
         <v>12</v>
       </c>
       <c r="F33" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A33,"0")," - ","CCMA - ",YEAR(F33)&amp;TEXT(MONTH(F33),"00")," - ",SUBSTITUTE(D33,"-","")," - ",B33)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I33" s="4" t="str">
@@ -3488,29 +3488,29 @@
         <v/>
       </c>
       <c r="J33" s="5" t="str">
-        <f>IF(EXACT(I33,E33),"ü","x")</f>
+        <f t="shared" si="2"/>
         <v>x</v>
       </c>
       <c r="K33" s="4">
-        <f>ROW(A33)</f>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="L33" s="4">
-        <f>IF(C33=C32,1,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M33" s="4">
-        <f>IF(C33=C34,1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N33" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="str">
-        <f t="shared" ref="A34:A69" si="4">RIGHT(D34,1)</f>
+        <f t="shared" ref="A34:A69" si="9">RIGHT(D34,1)</f>
         <v>0</v>
       </c>
       <c r="B34" t="s">
@@ -3526,12 +3526,12 @@
         <v>12</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A34,"0")," - ","CCMA - ",YEAR(F34)&amp;TEXT(MONTH(F34),"00")," - ",SUBSTITUTE(D34,"-","")," - ",B34)</f>
+        <f t="shared" ref="H34:H69" ca="1" si="10">CONCATENATE(TEXT(A34,"0")," - ","CCMA - ",YEAR(F34)&amp;TEXT(MONTH(F34),"00")," - ",SUBSTITUTE(D34,"-","")," - ",B34)</f>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I34" s="4" t="str">
@@ -3539,29 +3539,29 @@
         <v/>
       </c>
       <c r="J34" s="5" t="str">
-        <f>IF(EXACT(I34,E34),"ü","x")</f>
+        <f t="shared" ref="J34:J65" si="11">IF(EXACT(I34,E34),"ü","x")</f>
         <v>x</v>
       </c>
       <c r="K34" s="4">
-        <f>ROW(A34)</f>
+        <f t="shared" ref="K34:K69" si="12">ROW(A34)</f>
         <v>34</v>
       </c>
       <c r="L34" s="4">
-        <f>IF(C34=C33,1,0)</f>
+        <f t="shared" ref="L34:L69" si="13">IF(C34=C33,1,0)</f>
         <v>1</v>
       </c>
       <c r="M34" s="4">
-        <f>IF(C34=C35,1,0)</f>
+        <f t="shared" ref="M34:M69" si="14">IF(C34=C35,1,0)</f>
         <v>1</v>
       </c>
       <c r="N34" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B35" t="s">
@@ -3577,12 +3577,12 @@
         <v>12</v>
       </c>
       <c r="F35" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A35,"0")," - ","CCMA - ",YEAR(F35)&amp;TEXT(MONTH(F35),"00")," - ",SUBSTITUTE(D35,"-","")," - ",B35)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I35" s="4" t="str">
@@ -3590,29 +3590,29 @@
         <v/>
       </c>
       <c r="J35" s="5" t="str">
-        <f>IF(EXACT(I35,E35),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K35" s="4">
-        <f>ROW(A35)</f>
+        <f t="shared" si="12"/>
         <v>35</v>
       </c>
       <c r="L35" s="4">
-        <f>IF(C35=C34,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M35" s="4">
-        <f>IF(C35=C36,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N35" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B36" t="s">
@@ -3628,12 +3628,12 @@
         <v>12</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A36,"0")," - ","CCMA - ",YEAR(F36)&amp;TEXT(MONTH(F36),"00")," - ",SUBSTITUTE(D36,"-","")," - ",B36)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I36" s="4" t="str">
@@ -3641,29 +3641,29 @@
         <v/>
       </c>
       <c r="J36" s="5" t="str">
-        <f>IF(EXACT(I36,E36),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K36" s="4">
-        <f>ROW(A36)</f>
+        <f t="shared" si="12"/>
         <v>36</v>
       </c>
       <c r="L36" s="4">
-        <f>IF(C36=C35,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M36" s="4">
-        <f>IF(C36=C37,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N36" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B37" t="s">
@@ -3679,12 +3679,12 @@
         <v>12</v>
       </c>
       <c r="F37" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A37,"0")," - ","CCMA - ",YEAR(F37)&amp;TEXT(MONTH(F37),"00")," - ",SUBSTITUTE(D37,"-","")," - ",B37)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I37" s="4" t="str">
@@ -3692,29 +3692,29 @@
         <v/>
       </c>
       <c r="J37" s="5" t="str">
-        <f>IF(EXACT(I37,E37),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K37" s="4">
-        <f>ROW(A37)</f>
+        <f t="shared" si="12"/>
         <v>37</v>
       </c>
       <c r="L37" s="4">
-        <f>IF(C37=C36,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M37" s="4">
-        <f>IF(C37=C38,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N37" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B38" t="s">
@@ -3730,12 +3730,12 @@
         <v>12</v>
       </c>
       <c r="F38" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A38,"0")," - ","CCMA - ",YEAR(F38)&amp;TEXT(MONTH(F38),"00")," - ",SUBSTITUTE(D38,"-","")," - ",B38)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I38" s="4" t="str">
@@ -3743,29 +3743,29 @@
         <v/>
       </c>
       <c r="J38" s="5" t="str">
-        <f>IF(EXACT(I38,E38),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K38" s="4">
-        <f>ROW(A38)</f>
+        <f t="shared" si="12"/>
         <v>38</v>
       </c>
       <c r="L38" s="4">
-        <f>IF(C38=C37,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M38" s="4">
-        <f>IF(C38=C39,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N38" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B39" t="s">
@@ -3781,12 +3781,12 @@
         <v>12</v>
       </c>
       <c r="F39" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A39,"0")," - ","CCMA - ",YEAR(F39)&amp;TEXT(MONTH(F39),"00")," - ",SUBSTITUTE(D39,"-","")," - ",B39)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I39" s="4" t="str">
@@ -3794,29 +3794,29 @@
         <v/>
       </c>
       <c r="J39" s="5" t="str">
-        <f>IF(EXACT(I39,E39),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K39" s="4">
-        <f>ROW(A39)</f>
+        <f t="shared" si="12"/>
         <v>39</v>
       </c>
       <c r="L39" s="4">
-        <f>IF(C39=C38,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M39" s="4">
-        <f>IF(C39=C40,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N39" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B40" t="s">
@@ -3832,12 +3832,12 @@
         <v>12</v>
       </c>
       <c r="F40" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A40,"0")," - ","CCMA - ",YEAR(F40)&amp;TEXT(MONTH(F40),"00")," - ",SUBSTITUTE(D40,"-","")," - ",B40)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I40" s="4" t="str">
@@ -3845,29 +3845,29 @@
         <v/>
       </c>
       <c r="J40" s="5" t="str">
-        <f>IF(EXACT(I40,E40),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K40" s="4">
-        <f>ROW(A40)</f>
+        <f t="shared" si="12"/>
         <v>40</v>
       </c>
       <c r="L40" s="4">
-        <f>IF(C40=C39,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M40" s="4">
-        <f>IF(C40=C41,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N40" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B41" t="s">
@@ -3883,12 +3883,12 @@
         <v>12</v>
       </c>
       <c r="F41" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A41,"0")," - ","CCMA - ",YEAR(F41)&amp;TEXT(MONTH(F41),"00")," - ",SUBSTITUTE(D41,"-","")," - ",B41)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I41" s="4" t="str">
@@ -3896,29 +3896,29 @@
         <v/>
       </c>
       <c r="J41" s="5" t="str">
-        <f>IF(EXACT(I41,E41),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K41" s="4">
-        <f>ROW(A41)</f>
+        <f t="shared" si="12"/>
         <v>41</v>
       </c>
       <c r="L41" s="4">
-        <f>IF(C41=C40,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M41" s="4">
-        <f>IF(C41=C42,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N41" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B42" t="s">
@@ -3934,12 +3934,12 @@
         <v>12</v>
       </c>
       <c r="F42" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A42,"0")," - ","CCMA - ",YEAR(F42)&amp;TEXT(MONTH(F42),"00")," - ",SUBSTITUTE(D42,"-","")," - ",B42)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I42" s="4" t="str">
@@ -3947,29 +3947,29 @@
         <v/>
       </c>
       <c r="J42" s="5" t="str">
-        <f>IF(EXACT(I42,E42),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K42" s="4">
-        <f>ROW(A42)</f>
+        <f t="shared" si="12"/>
         <v>42</v>
       </c>
       <c r="L42" s="4">
-        <f>IF(C42=C41,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M42" s="4">
-        <f>IF(C42=C43,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N42" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B43" t="s">
@@ -3985,12 +3985,12 @@
         <v>12</v>
       </c>
       <c r="F43" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A43,"0")," - ","CCMA - ",YEAR(F43)&amp;TEXT(MONTH(F43),"00")," - ",SUBSTITUTE(D43,"-","")," - ",B43)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I43" s="4" t="str">
@@ -3998,29 +3998,29 @@
         <v/>
       </c>
       <c r="J43" s="5" t="str">
-        <f>IF(EXACT(I43,E43),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K43" s="4">
-        <f>ROW(A43)</f>
+        <f t="shared" si="12"/>
         <v>43</v>
       </c>
       <c r="L43" s="4">
-        <f>IF(C43=C42,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M43" s="4">
-        <f>IF(C43=C44,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N43" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B44" t="s">
@@ -4036,12 +4036,12 @@
         <v>12</v>
       </c>
       <c r="F44" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A44,"0")," - ","CCMA - ",YEAR(F44)&amp;TEXT(MONTH(F44),"00")," - ",SUBSTITUTE(D44,"-","")," - ",B44)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I44" s="4" t="str">
@@ -4049,29 +4049,29 @@
         <v/>
       </c>
       <c r="J44" s="5" t="str">
-        <f>IF(EXACT(I44,E44),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K44" s="4">
-        <f>ROW(A44)</f>
+        <f t="shared" si="12"/>
         <v>44</v>
       </c>
       <c r="L44" s="4">
-        <f>IF(C44=C43,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M44" s="4">
-        <f>IF(C44=C45,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N44" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B45" t="s">
@@ -4087,12 +4087,12 @@
         <v>12</v>
       </c>
       <c r="F45" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A45,"0")," - ","CCMA - ",YEAR(F45)&amp;TEXT(MONTH(F45),"00")," - ",SUBSTITUTE(D45,"-","")," - ",B45)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I45" s="4" t="str">
@@ -4100,29 +4100,29 @@
         <v/>
       </c>
       <c r="J45" s="5" t="str">
-        <f>IF(EXACT(I45,E45),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K45" s="4">
-        <f>ROW(A45)</f>
+        <f t="shared" si="12"/>
         <v>45</v>
       </c>
       <c r="L45" s="4">
-        <f>IF(C45=C44,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M45" s="4">
-        <f>IF(C45=C46,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N45" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B46" t="s">
@@ -4138,12 +4138,12 @@
         <v>12</v>
       </c>
       <c r="F46" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A46,"0")," - ","CCMA - ",YEAR(F46)&amp;TEXT(MONTH(F46),"00")," - ",SUBSTITUTE(D46,"-","")," - ",B46)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I46" s="4" t="str">
@@ -4151,29 +4151,29 @@
         <v/>
       </c>
       <c r="J46" s="5" t="str">
-        <f>IF(EXACT(I46,E46),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K46" s="4">
-        <f>ROW(A46)</f>
+        <f t="shared" si="12"/>
         <v>46</v>
       </c>
       <c r="L46" s="4">
-        <f>IF(C46=C45,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M46" s="4">
-        <f>IF(C46=C47,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N46" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B47" t="s">
@@ -4189,12 +4189,12 @@
         <v>12</v>
       </c>
       <c r="F47" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A47,"0")," - ","CCMA - ",YEAR(F47)&amp;TEXT(MONTH(F47),"00")," - ",SUBSTITUTE(D47,"-","")," - ",B47)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I47" s="4" t="str">
@@ -4202,29 +4202,29 @@
         <v/>
       </c>
       <c r="J47" s="5" t="str">
-        <f>IF(EXACT(I47,E47),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K47" s="4">
-        <f>ROW(A47)</f>
+        <f t="shared" si="12"/>
         <v>47</v>
       </c>
       <c r="L47" s="4">
-        <f>IF(C47=C46,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M47" s="4">
-        <f>IF(C47=C48,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N47" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B48" t="s">
@@ -4240,12 +4240,12 @@
         <v>12</v>
       </c>
       <c r="F48" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A48,"0")," - ","CCMA - ",YEAR(F48)&amp;TEXT(MONTH(F48),"00")," - ",SUBSTITUTE(D48,"-","")," - ",B48)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I48" s="4" t="str">
@@ -4253,29 +4253,29 @@
         <v/>
       </c>
       <c r="J48" s="5" t="str">
-        <f>IF(EXACT(I48,E48),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K48" s="4">
-        <f>ROW(A48)</f>
+        <f t="shared" si="12"/>
         <v>48</v>
       </c>
       <c r="L48" s="4">
-        <f>IF(C48=C47,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M48" s="4">
-        <f>IF(C48=C49,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N48" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B49" t="s">
@@ -4291,12 +4291,12 @@
         <v>12</v>
       </c>
       <c r="F49" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A49,"0")," - ","CCMA - ",YEAR(F49)&amp;TEXT(MONTH(F49),"00")," - ",SUBSTITUTE(D49,"-","")," - ",B49)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I49" s="4" t="str">
@@ -4304,29 +4304,29 @@
         <v/>
       </c>
       <c r="J49" s="5" t="str">
-        <f>IF(EXACT(I49,E49),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K49" s="4">
-        <f>ROW(A49)</f>
+        <f t="shared" si="12"/>
         <v>49</v>
       </c>
       <c r="L49" s="4">
-        <f>IF(C49=C48,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M49" s="4">
-        <f>IF(C49=C50,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N49" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B50" t="s">
@@ -4342,12 +4342,12 @@
         <v>12</v>
       </c>
       <c r="F50" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A50,"0")," - ","CCMA - ",YEAR(F50)&amp;TEXT(MONTH(F50),"00")," - ",SUBSTITUTE(D50,"-","")," - ",B50)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I50" s="4" t="str">
@@ -4355,29 +4355,29 @@
         <v/>
       </c>
       <c r="J50" s="5" t="str">
-        <f>IF(EXACT(I50,E50),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K50" s="4">
-        <f>ROW(A50)</f>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
       <c r="L50" s="4">
-        <f>IF(C50=C49,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M50" s="4">
-        <f>IF(C50=C51,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N50" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B51" t="s">
@@ -4393,12 +4393,12 @@
         <v>12</v>
       </c>
       <c r="F51" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A51,"0")," - ","CCMA - ",YEAR(F51)&amp;TEXT(MONTH(F51),"00")," - ",SUBSTITUTE(D51,"-","")," - ",B51)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I51" s="4" t="str">
@@ -4406,29 +4406,29 @@
         <v/>
       </c>
       <c r="J51" s="5" t="str">
-        <f>IF(EXACT(I51,E51),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K51" s="4">
-        <f>ROW(A51)</f>
+        <f t="shared" si="12"/>
         <v>51</v>
       </c>
       <c r="L51" s="4">
-        <f>IF(C51=C50,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M51" s="4">
-        <f>IF(C51=C52,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N51" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B52" t="s">
@@ -4444,12 +4444,12 @@
         <v>12</v>
       </c>
       <c r="F52" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G52" s="3"/>
       <c r="H52" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A52,"0")," - ","CCMA - ",YEAR(F52)&amp;TEXT(MONTH(F52),"00")," - ",SUBSTITUTE(D52,"-","")," - ",B52)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I52" s="4" t="str">
@@ -4457,29 +4457,29 @@
         <v/>
       </c>
       <c r="J52" s="5" t="str">
-        <f>IF(EXACT(I52,E52),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K52" s="4">
-        <f>ROW(A52)</f>
+        <f t="shared" si="12"/>
         <v>52</v>
       </c>
       <c r="L52" s="4">
-        <f>IF(C52=C51,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M52" s="4">
-        <f>IF(C52=C53,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N52" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B53" t="s">
@@ -4495,12 +4495,12 @@
         <v>12</v>
       </c>
       <c r="F53" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G53" s="3"/>
       <c r="H53" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A53,"0")," - ","CCMA - ",YEAR(F53)&amp;TEXT(MONTH(F53),"00")," - ",SUBSTITUTE(D53,"-","")," - ",B53)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I53" s="4" t="str">
@@ -4508,29 +4508,29 @@
         <v/>
       </c>
       <c r="J53" s="5" t="str">
-        <f>IF(EXACT(I53,E53),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K53" s="4">
-        <f>ROW(A53)</f>
+        <f t="shared" si="12"/>
         <v>53</v>
       </c>
       <c r="L53" s="4">
-        <f>IF(C53=C52,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M53" s="4">
-        <f>IF(C53=C54,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N53" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B54" t="s">
@@ -4546,12 +4546,12 @@
         <v>12</v>
       </c>
       <c r="F54" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G54" s="3"/>
       <c r="H54" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A54,"0")," - ","CCMA - ",YEAR(F54)&amp;TEXT(MONTH(F54),"00")," - ",SUBSTITUTE(D54,"-","")," - ",B54)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I54" s="4" t="str">
@@ -4559,29 +4559,29 @@
         <v/>
       </c>
       <c r="J54" s="5" t="str">
-        <f>IF(EXACT(I54,E54),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K54" s="4">
-        <f>ROW(A54)</f>
+        <f t="shared" si="12"/>
         <v>54</v>
       </c>
       <c r="L54" s="4">
-        <f>IF(C54=C53,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M54" s="4">
-        <f>IF(C54=C55,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N54" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B55" t="s">
@@ -4597,12 +4597,12 @@
         <v>12</v>
       </c>
       <c r="F55" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G55" s="3"/>
       <c r="H55" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A55,"0")," - ","CCMA - ",YEAR(F55)&amp;TEXT(MONTH(F55),"00")," - ",SUBSTITUTE(D55,"-","")," - ",B55)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I55" s="4" t="str">
@@ -4610,29 +4610,29 @@
         <v/>
       </c>
       <c r="J55" s="5" t="str">
-        <f>IF(EXACT(I55,E55),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K55" s="4">
-        <f>ROW(A55)</f>
+        <f t="shared" si="12"/>
         <v>55</v>
       </c>
       <c r="L55" s="4">
-        <f>IF(C55=C54,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M55" s="4">
-        <f>IF(C55=C56,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N55" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B56" t="s">
@@ -4648,12 +4648,12 @@
         <v>12</v>
       </c>
       <c r="F56" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G56" s="3"/>
       <c r="H56" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A56,"0")," - ","CCMA - ",YEAR(F56)&amp;TEXT(MONTH(F56),"00")," - ",SUBSTITUTE(D56,"-","")," - ",B56)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I56" s="4" t="str">
@@ -4661,29 +4661,29 @@
         <v/>
       </c>
       <c r="J56" s="5" t="str">
-        <f>IF(EXACT(I56,E56),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K56" s="4">
-        <f>ROW(A56)</f>
+        <f t="shared" si="12"/>
         <v>56</v>
       </c>
       <c r="L56" s="4">
-        <f>IF(C56=C55,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M56" s="4">
-        <f>IF(C56=C57,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N56" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B57" t="s">
@@ -4699,12 +4699,12 @@
         <v>12</v>
       </c>
       <c r="F57" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A57,"0")," - ","CCMA - ",YEAR(F57)&amp;TEXT(MONTH(F57),"00")," - ",SUBSTITUTE(D57,"-","")," - ",B57)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I57" s="4" t="str">
@@ -4712,29 +4712,29 @@
         <v/>
       </c>
       <c r="J57" s="5" t="str">
-        <f>IF(EXACT(I57,E57),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K57" s="4">
-        <f>ROW(A57)</f>
+        <f t="shared" si="12"/>
         <v>57</v>
       </c>
       <c r="L57" s="4">
-        <f>IF(C57=C56,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M57" s="4">
-        <f>IF(C57=C58,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N57" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B58" t="s">
@@ -4750,12 +4750,12 @@
         <v>12</v>
       </c>
       <c r="F58" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A58,"0")," - ","CCMA - ",YEAR(F58)&amp;TEXT(MONTH(F58),"00")," - ",SUBSTITUTE(D58,"-","")," - ",B58)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I58" s="4" t="str">
@@ -4763,29 +4763,29 @@
         <v/>
       </c>
       <c r="J58" s="5" t="str">
-        <f>IF(EXACT(I58,E58),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K58" s="4">
-        <f>ROW(A58)</f>
+        <f t="shared" si="12"/>
         <v>58</v>
       </c>
       <c r="L58" s="4">
-        <f>IF(C58=C57,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M58" s="4">
-        <f>IF(C58=C59,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N58" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B59" t="s">
@@ -4801,12 +4801,12 @@
         <v>12</v>
       </c>
       <c r="F59" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G59" s="3"/>
       <c r="H59" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A59,"0")," - ","CCMA - ",YEAR(F59)&amp;TEXT(MONTH(F59),"00")," - ",SUBSTITUTE(D59,"-","")," - ",B59)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I59" s="4" t="str">
@@ -4814,29 +4814,29 @@
         <v/>
       </c>
       <c r="J59" s="5" t="str">
-        <f>IF(EXACT(I59,E59),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K59" s="4">
-        <f>ROW(A59)</f>
+        <f t="shared" si="12"/>
         <v>59</v>
       </c>
       <c r="L59" s="4">
-        <f>IF(C59=C58,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M59" s="4">
-        <f>IF(C59=C60,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N59" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B60" t="s">
@@ -4852,12 +4852,12 @@
         <v>12</v>
       </c>
       <c r="F60" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A60,"0")," - ","CCMA - ",YEAR(F60)&amp;TEXT(MONTH(F60),"00")," - ",SUBSTITUTE(D60,"-","")," - ",B60)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I60" s="4" t="str">
@@ -4865,29 +4865,29 @@
         <v/>
       </c>
       <c r="J60" s="5" t="str">
-        <f>IF(EXACT(I60,E60),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K60" s="4">
-        <f>ROW(A60)</f>
+        <f t="shared" si="12"/>
         <v>60</v>
       </c>
       <c r="L60" s="4">
-        <f>IF(C60=C59,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M60" s="4">
-        <f>IF(C60=C61,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N60" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B61" t="s">
@@ -4903,12 +4903,12 @@
         <v>12</v>
       </c>
       <c r="F61" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G61" s="3"/>
       <c r="H61" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A61,"0")," - ","CCMA - ",YEAR(F61)&amp;TEXT(MONTH(F61),"00")," - ",SUBSTITUTE(D61,"-","")," - ",B61)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I61" s="4" t="str">
@@ -4916,29 +4916,29 @@
         <v/>
       </c>
       <c r="J61" s="5" t="str">
-        <f>IF(EXACT(I61,E61),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K61" s="4">
-        <f>ROW(A61)</f>
+        <f t="shared" si="12"/>
         <v>61</v>
       </c>
       <c r="L61" s="4">
-        <f>IF(C61=C60,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M61" s="4">
-        <f>IF(C61=C62,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N61" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B62" t="s">
@@ -4954,12 +4954,12 @@
         <v>12</v>
       </c>
       <c r="F62" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G62" s="3"/>
       <c r="H62" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A62,"0")," - ","CCMA - ",YEAR(F62)&amp;TEXT(MONTH(F62),"00")," - ",SUBSTITUTE(D62,"-","")," - ",B62)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I62" s="4" t="str">
@@ -4967,29 +4967,29 @@
         <v/>
       </c>
       <c r="J62" s="5" t="str">
-        <f>IF(EXACT(I62,E62),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K62" s="4">
-        <f>ROW(A62)</f>
+        <f t="shared" si="12"/>
         <v>62</v>
       </c>
       <c r="L62" s="4">
-        <f>IF(C62=C61,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M62" s="4">
-        <f>IF(C62=C63,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N62" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B63" t="s">
@@ -5005,12 +5005,12 @@
         <v>12</v>
       </c>
       <c r="F63" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G63" s="3"/>
       <c r="H63" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A63,"0")," - ","CCMA - ",YEAR(F63)&amp;TEXT(MONTH(F63),"00")," - ",SUBSTITUTE(D63,"-","")," - ",B63)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I63" s="4" t="str">
@@ -5018,29 +5018,29 @@
         <v/>
       </c>
       <c r="J63" s="5" t="str">
-        <f>IF(EXACT(I63,E63),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K63" s="4">
-        <f>ROW(A63)</f>
+        <f t="shared" si="12"/>
         <v>63</v>
       </c>
       <c r="L63" s="4">
-        <f>IF(C63=C62,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M63" s="4">
-        <f>IF(C63=C64,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N63" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B64" t="s">
@@ -5056,12 +5056,12 @@
         <v>12</v>
       </c>
       <c r="F64" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G64" s="3"/>
       <c r="H64" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A64,"0")," - ","CCMA - ",YEAR(F64)&amp;TEXT(MONTH(F64),"00")," - ",SUBSTITUTE(D64,"-","")," - ",B64)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I64" s="4" t="str">
@@ -5069,29 +5069,29 @@
         <v/>
       </c>
       <c r="J64" s="5" t="str">
-        <f>IF(EXACT(I64,E64),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K64" s="4">
-        <f>ROW(A64)</f>
+        <f t="shared" si="12"/>
         <v>64</v>
       </c>
       <c r="L64" s="4">
-        <f>IF(C64=C63,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M64" s="4">
-        <f>IF(C64=C65,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N64" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B65" t="s">
@@ -5107,12 +5107,12 @@
         <v>12</v>
       </c>
       <c r="F65" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A65,"0")," - ","CCMA - ",YEAR(F65)&amp;TEXT(MONTH(F65),"00")," - ",SUBSTITUTE(D65,"-","")," - ",B65)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I65" s="4" t="str">
@@ -5120,29 +5120,29 @@
         <v/>
       </c>
       <c r="J65" s="5" t="str">
-        <f>IF(EXACT(I65,E65),"ü","x")</f>
+        <f t="shared" si="11"/>
         <v>x</v>
       </c>
       <c r="K65" s="4">
-        <f>ROW(A65)</f>
+        <f t="shared" si="12"/>
         <v>65</v>
       </c>
       <c r="L65" s="4">
-        <f>IF(C65=C64,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M65" s="4">
-        <f>IF(C65=C66,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N65" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B66" t="s">
@@ -5158,12 +5158,12 @@
         <v>12</v>
       </c>
       <c r="F66" s="3">
-        <f t="shared" ca="1" si="2"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>45132</v>
       </c>
       <c r="G66" s="3"/>
       <c r="H66" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A66,"0")," - ","CCMA - ",YEAR(F66)&amp;TEXT(MONTH(F66),"00")," - ",SUBSTITUTE(D66,"-","")," - ",B66)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I66" s="4" t="str">
@@ -5171,29 +5171,29 @@
         <v/>
       </c>
       <c r="J66" s="5" t="str">
-        <f>IF(EXACT(I66,E66),"ü","x")</f>
+        <f t="shared" ref="J66:J97" si="15">IF(EXACT(I66,E66),"ü","x")</f>
         <v>x</v>
       </c>
       <c r="K66" s="4">
-        <f>ROW(A66)</f>
+        <f t="shared" si="12"/>
         <v>66</v>
       </c>
       <c r="L66" s="4">
-        <f>IF(C66=C65,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M66" s="4">
-        <f>IF(C66=C67,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N66" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B67" t="s">
@@ -5209,12 +5209,12 @@
         <v>12</v>
       </c>
       <c r="F67" s="3">
-        <f t="shared" ref="F67:F69" ca="1" si="5">TODAY()</f>
-        <v>45131</v>
+        <f t="shared" ref="F67:F69" ca="1" si="16">TODAY()</f>
+        <v>45132</v>
       </c>
       <c r="G67" s="3"/>
       <c r="H67" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A67,"0")," - ","CCMA - ",YEAR(F67)&amp;TEXT(MONTH(F67),"00")," - ",SUBSTITUTE(D67,"-","")," - ",B67)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I67" s="4" t="str">
@@ -5222,29 +5222,29 @@
         <v/>
       </c>
       <c r="J67" s="5" t="str">
-        <f>IF(EXACT(I67,E67),"ü","x")</f>
+        <f t="shared" si="15"/>
         <v>x</v>
       </c>
       <c r="K67" s="4">
-        <f>ROW(A67)</f>
+        <f t="shared" si="12"/>
         <v>67</v>
       </c>
       <c r="L67" s="4">
-        <f>IF(C67=C66,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M67" s="4">
-        <f>IF(C67=C68,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N67" s="4">
-        <f t="shared" ref="N67:N69" si="6">SUM(L67:M67)</f>
+        <f t="shared" ref="N67:N69" si="17">SUM(L67:M67)</f>
         <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B68" t="s">
@@ -5260,12 +5260,12 @@
         <v>12</v>
       </c>
       <c r="F68" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>45132</v>
       </c>
       <c r="G68" s="3"/>
       <c r="H68" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A68,"0")," - ","CCMA - ",YEAR(F68)&amp;TEXT(MONTH(F68),"00")," - ",SUBSTITUTE(D68,"-","")," - ",B68)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I68" s="4" t="str">
@@ -5273,29 +5273,29 @@
         <v/>
       </c>
       <c r="J68" s="5" t="str">
-        <f>IF(EXACT(I68,E68),"ü","x")</f>
+        <f t="shared" si="15"/>
         <v>x</v>
       </c>
       <c r="K68" s="4">
-        <f>ROW(A68)</f>
+        <f t="shared" si="12"/>
         <v>68</v>
       </c>
       <c r="L68" s="4">
-        <f>IF(C68=C67,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M68" s="4">
-        <f>IF(C68=C69,1,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="N68" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="B69" t="s">
@@ -5311,12 +5311,12 @@
         <v>12</v>
       </c>
       <c r="F69" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>45131</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>45132</v>
       </c>
       <c r="G69" s="3"/>
       <c r="H69" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A69,"0")," - ","CCMA - ",YEAR(F69)&amp;TEXT(MONTH(F69),"00")," - ",SUBSTITUTE(D69,"-","")," - ",B69)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>0 - CCMA - 202307 - 30000000000 - Cliente</v>
       </c>
       <c r="I69" s="4" t="str">
@@ -5324,23 +5324,23 @@
         <v/>
       </c>
       <c r="J69" s="5" t="str">
-        <f>IF(EXACT(I69,E69),"ü","x")</f>
+        <f t="shared" si="15"/>
         <v>x</v>
       </c>
       <c r="K69" s="4">
-        <f>ROW(A69)</f>
+        <f t="shared" si="12"/>
         <v>69</v>
       </c>
       <c r="L69" s="4">
-        <f>IF(C69=C68,1,0)</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="M69" s="4">
-        <f>IF(C69=C70,1,0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N69" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>